<commit_message>
move excel files, fix Java CI
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -1070,6 +1070,9 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1082,6 +1085,12 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1111,15 +1120,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2098,36 +2098,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="88" t="s">
+      <c r="F1" s="92"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="88" t="s">
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="89"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="93" t="s">
+      <c r="L1" s="92"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="88" t="s">
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="89"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="88" t="s">
+      <c r="R1" s="92"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="89"/>
-      <c r="V1" s="90"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="93"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2517,31 +2517,31 @@
       <c r="D3" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="89"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88" t="s">
+      <c r="F3" s="92"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="88" t="s">
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="89"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="93" t="s">
+      <c r="L3" s="92"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="88" t="s">
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="89"/>
-      <c r="S3" s="90"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="93"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
@@ -3667,7 +3667,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3683,41 +3683,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="96" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="80" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="82"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -3776,10 +3776,10 @@
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
       <c r="A5" s="63"/>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="84"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -3992,11 +3992,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
@@ -4025,7 +4025,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="87" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -4051,7 +4051,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="84"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
@@ -4075,7 +4075,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="84"/>
+      <c r="A7" s="87"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
@@ -4099,7 +4099,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="84"/>
+      <c r="A8" s="87"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
@@ -4123,7 +4123,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="88" t="s">
         <v>172</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -4144,7 +4144,7 @@
       <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="85"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="23" t="s">
         <v>152</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="85"/>
+      <c r="A11" s="88"/>
       <c r="B11" s="23" t="s">
         <v>153</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="85"/>
+      <c r="A12" s="88"/>
       <c r="B12" s="23" t="s">
         <v>154</v>
       </c>
@@ -4206,7 +4206,7 @@
       <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="85"/>
+      <c r="A13" s="88"/>
       <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
@@ -4315,31 +4315,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="88" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="88" t="s">
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="89"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91" t="s">
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="88" t="s">
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="90"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="93"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4660,26 +4660,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="88" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="88" t="s">
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="89"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91" t="s">
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
add version into BDD excel
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/BDDExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDD96103-1865-41AC-AC4F-6F41B3C4A984}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3210D8EB-9027-4CD9-B2FA-25E823394580}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
-    <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
+    <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="177">
   <si>
     <t>Role</t>
   </si>
@@ -564,6 +564,18 @@
   </si>
   <si>
     <t>Get data from Excel, then check</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>V0.1</t>
+  </si>
+  <si>
+    <t>V0.2</t>
+  </si>
+  <si>
+    <t>check data area</t>
   </si>
 </sst>
 </file>
@@ -636,7 +648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,12 +699,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,7 +963,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1094,9 +1099,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1120,6 +1122,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1633,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1644,14 +1652,15 @@
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45">
+    <row r="1" spans="1:9" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1661,23 +1670,26 @@
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1687,23 +1699,26 @@
       <c r="C2" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -1713,23 +1728,26 @@
       <c r="C3" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
         <v>2</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -1739,23 +1757,26 @@
       <c r="C4" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -1765,11 +1786,11 @@
       <c r="C5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>3</v>
@@ -1780,8 +1801,11 @@
       <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -1791,11 +1815,11 @@
       <c r="C6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>17</v>
@@ -1806,8 +1830,11 @@
       <c r="H6" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -1817,11 +1844,11 @@
       <c r="C7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4.4000000000000004</v>
       </c>
       <c r="F7" s="7">
         <v>4.4000000000000004</v>
@@ -1832,8 +1859,11 @@
       <c r="H7" s="7">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="30">
+      <c r="I7" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -1843,11 +1873,11 @@
       <c r="C8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>18</v>
@@ -1858,8 +1888,11 @@
       <c r="H8" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="30">
+      <c r="I8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -1869,11 +1902,11 @@
       <c r="C9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>22</v>
@@ -1884,8 +1917,11 @@
       <c r="H9" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="22">
         <v>9</v>
       </c>
@@ -1895,15 +1931,18 @@
       <c r="C10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" ht="30">
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" s="22">
         <v>10</v>
       </c>
@@ -1913,29 +1952,32 @@
       <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="44">
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="45">
+      <c r="A12" s="43">
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="47" t="s">
         <v>86</v>
-      </c>
-      <c r="E12" s="7">
-        <v>3</v>
       </c>
       <c r="F12" s="7">
         <v>3</v>
@@ -1946,44 +1988,56 @@
       <c r="H12" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="45"/>
+      <c r="I12" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="44"/>
       <c r="B13" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="48"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="45"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="44"/>
       <c r="B14" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="7"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" s="48"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="46"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="45"/>
       <c r="B15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" ht="30">
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="30">
       <c r="A16" s="25">
         <v>12</v>
       </c>
@@ -1993,11 +2047,11 @@
       <c r="C16" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>91</v>
@@ -2008,8 +2062,11 @@
       <c r="H16" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="30">
+      <c r="I16" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30">
       <c r="A17" s="25">
         <v>13</v>
       </c>
@@ -2019,11 +2076,11 @@
       <c r="C17" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="E17" s="7">
-        <v>5</v>
       </c>
       <c r="F17" s="7">
         <v>5</v>
@@ -2034,22 +2091,25 @@
       <c r="H17" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="42" t="s">
         <v>164</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4</v>
       </c>
       <c r="F18" s="7">
         <v>4</v>
@@ -2058,6 +2118,9 @@
         <v>4</v>
       </c>
       <c r="H18" s="7">
+        <v>4</v>
+      </c>
+      <c r="I18" s="7">
         <v>4</v>
       </c>
     </row>
@@ -2065,7 +2128,7 @@
   <mergeCells count="3">
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2098,36 +2161,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="91" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="92"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="91" t="s">
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="92"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="96" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="91" t="s">
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="92"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="91" t="s">
+      <c r="R1" s="90"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="92"/>
-      <c r="V1" s="93"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="91"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2517,31 +2580,31 @@
       <c r="D3" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="91" t="s">
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="91" t="s">
+      <c r="I3" s="90"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="92"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="96" t="s">
+      <c r="L3" s="90"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="91" t="s">
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="92"/>
-      <c r="S3" s="93"/>
+      <c r="R3" s="90"/>
+      <c r="S3" s="91"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
@@ -2974,7 +3037,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2987,7 +3050,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -2998,7 +3061,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3021,7 +3084,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="54"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -3293,15 +3356,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -3337,7 +3400,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -3363,7 +3426,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -3387,7 +3450,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -3465,42 +3528,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="55"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="67" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="67"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -3532,16 +3595,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="61" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="55" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -3561,12 +3624,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="63"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="57"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -3584,12 +3647,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="63"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="58"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -3599,7 +3662,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="64"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -3666,7 +3729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -3683,41 +3746,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="81" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -3744,14 +3807,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="76"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75"/>
       <c r="E4" s="30" t="s">
         <v>103</v>
       </c>
@@ -3775,11 +3838,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="63"/>
-      <c r="B5" s="84" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="84"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -3806,12 +3869,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="63"/>
-      <c r="B6" s="77" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="79"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="30" t="s">
         <v>109</v>
       </c>
@@ -3835,11 +3898,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="63"/>
-      <c r="B7" s="68" t="s">
+      <c r="A7" s="62"/>
+      <c r="B7" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="69"/>
+      <c r="C7" s="68"/>
       <c r="D7" s="34" t="s">
         <v>114</v>
       </c>
@@ -3866,9 +3929,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="63"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="35" t="s">
         <v>120</v>
       </c>
@@ -3895,9 +3958,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="63"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="34" t="s">
         <v>121</v>
       </c>
@@ -3924,9 +3987,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="64"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="73"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="34" t="s">
         <v>122</v>
       </c>
@@ -3973,32 +4036,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
-  <dimension ref="A3:H17"/>
+  <dimension ref="A3:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8">
-      <c r="F3" s="89" t="s">
+    <row r="3" spans="1:9">
+      <c r="G3" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -4009,23 +4072,26 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="G4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="H4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="87" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="86" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -4034,96 +4100,108 @@
       <c r="C5" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="22">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="G5" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H5" s="41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="87"/>
+      <c r="I5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="86"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="22">
         <v>2</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="G6" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H6" s="41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="87"/>
+      <c r="I6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="86"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="22">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="40">
+      <c r="G7" s="40">
         <v>2</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="87"/>
+      <c r="I7" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="86"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="22">
         <v>4</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="G8" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H8" s="41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="88" t="s">
+      <c r="I8" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="95" t="s">
         <v>172</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -4132,159 +4210,231 @@
       <c r="C9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="22">
         <v>5</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="H9" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="41"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="88"/>
+      <c r="I9" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="95"/>
       <c r="B10" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="22">
         <v>6</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="G10" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="88"/>
+      <c r="I10" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="95"/>
       <c r="B11" s="23" t="s">
         <v>153</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="22">
         <v>7</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="G11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="41"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="88"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="95"/>
       <c r="B12" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="22">
         <v>8</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="G12" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="88"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="95"/>
       <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="22">
         <v>9</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="G13" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="41"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="E14" s="4" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="95"/>
+      <c r="B14" s="96" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="22">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="2" t="str">
-        <f>F14</f>
+      <c r="H14" s="2" t="str">
+        <f>G14</f>
         <v>V1.1</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="E15" s="4" t="s">
+      <c r="I14" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="95"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="22">
+        <v>11</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="2" t="str">
-        <f t="shared" ref="G15:G17" si="0">F15</f>
+      <c r="H15" s="2" t="str">
+        <f t="shared" ref="H15:H17" si="0">G15</f>
         <v>V2.1</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="E16" s="4" t="s">
+      <c r="I15" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="95"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="22">
+        <v>12</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8">
-      <c r="E17" s="4" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="95"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E17" s="22">
+        <v>13</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="2" t="str">
+      <c r="H17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>2021/4/30</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A9:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4315,31 +4465,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="91" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="91" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="94" t="s">
+      <c r="J1" s="90"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="91" t="s">
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="93"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4660,26 +4810,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="91" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="91" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="94" t="s">
+      <c r="J1" s="90"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -4800,12 +4950,12 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">

</xml_diff>

<commit_message>
add version column in BDD Excel
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/BDDExcel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3210D8EB-9027-4CD9-B2FA-25E823394580}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F164EB1C-D009-4843-BF95-D2EDB287610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="178">
   <si>
     <t>Role</t>
   </si>
@@ -576,6 +576,9 @@
   </si>
   <si>
     <t>check data area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario      </t>
   </si>
 </sst>
 </file>
@@ -877,7 +880,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1105,6 +1108,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1123,11 +1132,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2161,36 +2176,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="89" t="s">
+      <c r="F1" s="92"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="89" t="s">
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="90"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="94" t="s">
+      <c r="L1" s="92"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="89" t="s">
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="90"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="89" t="s">
+      <c r="R1" s="92"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="90"/>
-      <c r="V1" s="91"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="93"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2580,31 +2595,31 @@
       <c r="D3" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="F3" s="92"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="89" t="s">
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="90"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="94" t="s">
+      <c r="L3" s="92"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="89" t="s">
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="90"/>
-      <c r="S3" s="91"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="93"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
@@ -4039,7 +4054,7 @@
   <dimension ref="A3:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4055,6 +4070,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9">
+      <c r="A3" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="97" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="99" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="G3" s="87" t="s">
         <v>40</v>
       </c>
@@ -4062,21 +4095,11 @@
       <c r="I3" s="88"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>159</v>
-      </c>
+      <c r="A4" s="98"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
       <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
@@ -4201,7 +4224,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="90" t="s">
         <v>172</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -4227,7 +4250,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="95"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="23" t="s">
         <v>152</v>
       </c>
@@ -4254,7 +4277,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="95"/>
+      <c r="A11" s="90"/>
       <c r="B11" s="23" t="s">
         <v>153</v>
       </c>
@@ -4279,7 +4302,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="95"/>
+      <c r="A12" s="90"/>
       <c r="B12" s="23" t="s">
         <v>154</v>
       </c>
@@ -4304,7 +4327,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="95"/>
+      <c r="A13" s="90"/>
       <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
@@ -4329,8 +4352,8 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="95"/>
-      <c r="B14" s="96" t="s">
+      <c r="A14" s="90"/>
+      <c r="B14" s="89" t="s">
         <v>176</v>
       </c>
       <c r="C14" s="25" t="s">
@@ -4357,8 +4380,8 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="95"/>
-      <c r="B15" s="96"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="89"/>
       <c r="C15" s="25" t="s">
         <v>5</v>
       </c>
@@ -4383,8 +4406,8 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="95"/>
-      <c r="B16" s="96"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="25" t="s">
         <v>5</v>
       </c>
@@ -4404,8 +4427,8 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="95"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="89"/>
       <c r="C17" s="25" t="s">
         <v>5</v>
       </c>
@@ -4430,11 +4453,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="A9:A17"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4465,31 +4493,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="89" t="s">
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92" t="s">
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="89" t="s">
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="91"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="93"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4810,26 +4838,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="89" t="s">
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92" t="s">
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
use one function to handle expected and testresult
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F164EB1C-D009-4843-BF95-D2EDB287610C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6D387E-E5DE-4D17-9415-69020AF984C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
-    <sheet name="StoryExample1" sheetId="8" r:id="rId6"/>
-    <sheet name="SpecificationByTestcase" sheetId="9" r:id="rId7"/>
+    <sheet name="SpecificationByTestcase" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
+    <sheet name="StoryExample1" sheetId="8" r:id="rId7"/>
     <sheet name="SBTSheet1" sheetId="7" r:id="rId8"/>
     <sheet name="SBTSheet2" sheetId="10" r:id="rId9"/>
     <sheet name="SBTSheet3" sheetId="11" r:id="rId10"/>
-    <sheet name="SBTSheet3 (2)" sheetId="12" r:id="rId11"/>
+    <sheet name="Expected1" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="184">
   <si>
     <t>Role</t>
   </si>
@@ -579,6 +579,24 @@
   </si>
   <si>
     <t xml:space="preserve">Scenario      </t>
+  </si>
+  <si>
+    <t>Not match</t>
+  </si>
+  <si>
+    <t>Set Switch -Expected on</t>
+  </si>
+  <si>
+    <t>Set Switch -TestResult on</t>
+  </si>
+  <si>
+    <t>ExpectedSwitch</t>
+  </si>
+  <si>
+    <t>TestResultSwitch</t>
+  </si>
+  <si>
+    <t>On</t>
   </si>
 </sst>
 </file>
@@ -880,7 +898,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1108,12 +1126,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1132,18 +1159,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1298,55 +1323,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2419350" y="695325"/>
-          <a:ext cx="2932542" cy="2276475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3208767</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>2400300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F385B2A-A2CD-43B8-A7C4-46F10268F5C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2419350" y="1076325"/>
           <a:ext cx="2932542" cy="2276475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2176,36 +2152,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="91" t="s">
+      <c r="F1" s="95"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="92"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="91" t="s">
+      <c r="I1" s="95"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="92"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="96" t="s">
+      <c r="L1" s="95"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="91" t="s">
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="92"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="91" t="s">
+      <c r="R1" s="95"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="94" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="92"/>
-      <c r="V1" s="93"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="96"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2571,375 +2547,741 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2264DA-2ABC-4703-92C5-C6046C9B8A71}">
-  <dimension ref="A3:S13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFF208A-E752-404F-A219-18F91B0322F1}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:S8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19">
-      <c r="D3" s="37" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="C1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="91" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="91" t="s">
+      <c r="F1" s="95"/>
+      <c r="G1" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="92"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="96" t="s">
+      <c r="H1" s="95"/>
+      <c r="I1" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="91" t="s">
+      <c r="J1" s="98"/>
+      <c r="K1" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="92"/>
-      <c r="S3" s="93"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
+      <c r="L1" s="95"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>C3</f>
+        <v>V1.1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f>E3</f>
+        <v>V1.2</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f>G3</f>
+        <v>V1.3</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="8" t="str">
+        <f>I3</f>
+        <v>V1.4</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f>K3</f>
+        <v>V1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="M4" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="N4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="O4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="P4" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="R4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="S4" s="36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="9">
-        <v>1</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="8" t="str">
-        <f>E5</f>
-        <v>V1.1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="8" t="str">
-        <f>H5</f>
-        <v>V1.2</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="8" t="str">
-        <f>K5</f>
-        <v>V1.3</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="8" t="str">
-        <f>N5</f>
-        <v>V1.4</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="R5" s="8" t="str">
-        <f>Q5</f>
-        <v>V1.5</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="214.5" customHeight="1">
-      <c r="A6" s="9">
-        <v>2</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="8" t="str">
-        <f t="shared" ref="F6:F8" si="0">E6</f>
+      <c r="D4" s="8" t="str">
+        <f t="shared" ref="D4:D6" si="0">C4</f>
         <v>V2.1</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="8" t="str">
-        <f t="shared" ref="I6:I8" si="1">H6</f>
+      <c r="F4" s="8" t="str">
+        <f t="shared" ref="F4:F6" si="1">E4</f>
         <v>V2.2</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="K6" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="8" t="str">
-        <f t="shared" ref="L6:L8" si="2">K6</f>
+      <c r="H4" s="8" t="str">
+        <f t="shared" ref="H4:H6" si="2">G4</f>
         <v>V2.3</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="N6" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="8" t="str">
-        <f t="shared" ref="O6:O8" si="3">N6</f>
+      <c r="J4" s="8" t="str">
+        <f t="shared" ref="J4:J6" si="3">I4</f>
         <v>V2.4</v>
       </c>
-      <c r="P6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q6" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="R6" s="8" t="str">
-        <f t="shared" ref="R6" si="4">Q6</f>
+      <c r="L4" s="8" t="str">
+        <f t="shared" ref="L4" si="4">K4</f>
         <v>V2.5</v>
       </c>
-      <c r="S6" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="9">
-        <v>3</v>
-      </c>
-      <c r="B7" s="38" t="s">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="9">
-        <v>4</v>
-      </c>
-      <c r="B8" s="39" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="C6" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="8" t="str">
+      <c r="D6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>2021/4/30</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H8" s="8" t="b">
+      <c r="E6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="8" t="b">
+      <c r="F6" s="8" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="K8" s="28" t="b">
+      <c r="G6" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="L8" s="8" t="b">
+      <c r="H6" s="8" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="N8" s="7">
+      <c r="I6" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O8" s="8">
+      <c r="J6" s="8">
         <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q8" s="7">
+      <c r="K6" s="7">
         <v>5.4</v>
       </c>
-      <c r="R8" s="8">
-        <f t="shared" ref="R8" si="5">Q8</f>
+      <c r="L6" s="8">
+        <f t="shared" ref="L6" si="5">K6</f>
         <v>5.4</v>
       </c>
-      <c r="S8" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="D13" t="s">
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
         <v>87</v>
       </c>
-      <c r="E13" t="s">
+      <c r="C11" t="s">
         <v>88</v>
       </c>
-      <c r="F13" t="s">
+      <c r="D11" t="s">
         <v>88</v>
       </c>
-      <c r="G13" t="s">
+      <c r="E11" t="s">
         <v>88</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G11" t="s">
         <v>88</v>
       </c>
-      <c r="K13" t="s">
-        <v>88</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="I11" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
+  <dimension ref="A3:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9">
+      <c r="A3" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="90" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="92" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="92" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="86"/>
+      <c r="B6" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="86"/>
+      <c r="B7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="22">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="40">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="86"/>
+      <c r="B8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="22">
+        <v>4</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="86"/>
+      <c r="B9" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="22">
+        <v>5</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="86"/>
+      <c r="B10" s="101" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="22">
+        <v>6</v>
+      </c>
+      <c r="F10" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="H10" s="103" t="s">
+        <v>161</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="22">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="89"/>
+      <c r="B12" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="22">
+        <v>8</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="89"/>
+      <c r="B13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="22">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="89"/>
+      <c r="B14" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="22">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="89"/>
+      <c r="B15" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="22">
+        <v>11</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="89"/>
+      <c r="B16" s="100" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="22">
+        <v>12</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f>G16</f>
+        <v>V1.1</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="89"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E17" s="22">
+        <v>13</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f t="shared" ref="H17:H19" si="0">G17</f>
+        <v>V2.1</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="89"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="22">
+        <v>14</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="89"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="22">
+        <v>15</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5657C2-106C-47C7-BF16-329C2F267F09}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -3140,7 +3482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A494DA1E-3A4D-414E-886D-A717DFF21DE7}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -3354,7 +3696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3FD2D2-D808-401C-A638-EED224C6394A}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -3525,7 +3867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9F3738-1988-486F-BE99-D486460FE985}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -3740,7 +4082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -4049,426 +4391,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
-  <dimension ref="A3:I17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:9">
-      <c r="A3" s="97" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="97" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="99" t="s">
-        <v>173</v>
-      </c>
-      <c r="E3" s="99" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G3" s="87" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="98"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="22">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="86"/>
-      <c r="B6" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" s="22">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="86"/>
-      <c r="B7" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E7" s="22">
-        <v>3</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="40">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="86"/>
-      <c r="B8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="22">
-        <v>4</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
-      <c r="A9" s="90" t="s">
-        <v>172</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="22">
-        <v>5</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="90"/>
-      <c r="B10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" s="22">
-        <v>6</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="90"/>
-      <c r="B11" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" s="22">
-        <v>7</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="90"/>
-      <c r="B12" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="22">
-        <v>8</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="90"/>
-      <c r="B13" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13" s="22">
-        <v>9</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="90"/>
-      <c r="B14" s="89" t="s">
-        <v>176</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" s="22">
-        <v>10</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="2" t="str">
-        <f>G14</f>
-        <v>V1.1</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="90"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" s="22">
-        <v>11</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="2" t="str">
-        <f t="shared" ref="H15:H17" si="0">G15</f>
-        <v>V2.1</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="90"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="22">
-        <v>12</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="90"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E17" s="22">
-        <v>13</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>2021/4/30</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
   <dimension ref="A1:Q11"/>
@@ -4487,37 +4409,38 @@
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="91" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="91" t="s">
+      <c r="G1" s="95"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="94" t="s">
+      <c r="J1" s="95"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="91" t="s">
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="93"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="96"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4838,26 +4761,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="91" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="92"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="91" t="s">
+      <c r="G1" s="95"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="94" t="s">
+      <c r="J1" s="95"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
add test on expected - Azure46
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6D387E-E5DE-4D17-9415-69020AF984C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F01C691-C4EB-480A-B7D8-3EA5CE8BA071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="187">
   <si>
     <t>Role</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>On</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario5:Expected </t>
+  </si>
+  <si>
+    <t>Expected1</t>
   </si>
 </sst>
 </file>
@@ -988,6 +997,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1009,6 +1025,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1117,30 +1160,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1159,16 +1178,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1632,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1648,10 +1657,10 @@
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45">
+    <row r="1" spans="1:10" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1679,8 +1688,11 @@
       <c r="I1" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="30">
+      <c r="J1" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1708,8 +1720,11 @@
       <c r="I2" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -1717,7 +1732,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>174</v>
@@ -1737,8 +1752,11 @@
       <c r="I3" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+      <c r="J3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>174</v>
@@ -1766,71 +1784,76 @@
       <c r="I4" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
-      <c r="A5" s="22">
+      <c r="J4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="22"/>
+      <c r="B6" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30">
+      <c r="A7" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B7" s="23" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="22">
-        <v>5</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="22">
-        <v>6</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>35</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>5</v>
@@ -1839,27 +1862,30 @@
         <v>174</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G7" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H7" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I7" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30">
+        <v>39</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="22">
-        <v>7</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>69</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>5</v>
@@ -1868,27 +1894,30 @@
         <v>174</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="22">
-        <v>8</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>70</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>5</v>
@@ -1897,27 +1926,30 @@
         <v>174</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H9" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I9" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J9" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>5</v>
@@ -1926,19 +1958,30 @@
         <v>174</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+        <v>71</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30">
       <c r="A11" s="22">
-        <v>10</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>82</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>70</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>5</v>
@@ -1947,151 +1990,154 @@
         <v>174</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="45">
-      <c r="A12" s="43">
-        <v>11</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="22">
+        <v>9</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E12" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="7">
-        <v>3</v>
-      </c>
-      <c r="G12" s="7">
-        <v>3</v>
-      </c>
-      <c r="H12" s="7">
-        <v>3</v>
-      </c>
-      <c r="I12" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="44"/>
-      <c r="B13" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="46"/>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="30">
+      <c r="A13" s="22">
+        <v>10</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="48"/>
+      <c r="E13" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="44"/>
-      <c r="B14" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="46"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="45">
+      <c r="A14" s="46">
+        <v>11</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>5</v>
+      </c>
       <c r="D14" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="45"/>
-      <c r="B15" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="46"/>
+      <c r="E14" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="7">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7">
+        <v>3</v>
+      </c>
+      <c r="I14" s="7">
+        <v>3</v>
+      </c>
+      <c r="J14" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="47"/>
+      <c r="B15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="49"/>
       <c r="D15" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E15" s="49"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="30">
-      <c r="A16" s="25">
-        <v>12</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>5</v>
-      </c>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="47"/>
+      <c r="B16" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="49"/>
       <c r="D16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="25">
-        <v>13</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>5</v>
-      </c>
+      <c r="E16" s="51"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="48"/>
+      <c r="B17" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="49"/>
       <c r="D17" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="7">
-        <v>5</v>
-      </c>
-      <c r="G17" s="7">
-        <v>5</v>
-      </c>
-      <c r="H17" s="7">
-        <v>5</v>
-      </c>
-      <c r="I17" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="2">
-        <v>14</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>164</v>
+      <c r="E17" s="52"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="A18" s="25">
+        <v>12</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>5</v>
@@ -2099,27 +2145,94 @@
       <c r="D18" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" s="25">
+        <v>13</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="7">
+        <v>5</v>
+      </c>
+      <c r="G19" s="7">
+        <v>5</v>
+      </c>
+      <c r="H19" s="7">
+        <v>5</v>
+      </c>
+      <c r="I19" s="7">
+        <v>5</v>
+      </c>
+      <c r="J19" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2">
+        <v>14</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F20" s="7">
         <v>4</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G20" s="7">
         <v>4</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H20" s="7">
         <v>4</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I20" s="7">
         <v>4</v>
+      </c>
+      <c r="J20" s="7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="E14:E17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2152,36 +2265,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="94" t="s">
+      <c r="F1" s="99"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="95"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="94" t="s">
+      <c r="I1" s="99"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="95"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="99" t="s">
+      <c r="L1" s="99"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="94" t="s">
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="95"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="94" t="s">
+      <c r="R1" s="99"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="95"/>
-      <c r="V1" s="96"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="100"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2566,26 +2679,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="94" t="s">
+      <c r="D1" s="99"/>
+      <c r="E1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="94" t="s">
+      <c r="F1" s="99"/>
+      <c r="G1" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="95"/>
-      <c r="I1" s="97" t="s">
+      <c r="H1" s="99"/>
+      <c r="I1" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="98"/>
-      <c r="K1" s="94" t="s">
+      <c r="J1" s="102"/>
+      <c r="K1" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="95"/>
+      <c r="L1" s="99"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -2808,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
   <dimension ref="A3:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2826,36 +2939,36 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="60" t="s">
         <v>159</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
       <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
@@ -2870,7 +2983,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="53" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -2899,7 +3012,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="86"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
@@ -2926,7 +3039,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="86"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
@@ -2953,7 +3066,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="86"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
@@ -2980,7 +3093,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="86"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="23" t="s">
         <v>179</v>
       </c>
@@ -3007,8 +3120,8 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="86"/>
-      <c r="B10" s="101" t="s">
+      <c r="A10" s="53"/>
+      <c r="B10" s="43" t="s">
         <v>180</v>
       </c>
       <c r="C10" s="25" t="s">
@@ -3020,13 +3133,13 @@
       <c r="E10" s="22">
         <v>6</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="44" t="s">
         <v>182</v>
       </c>
       <c r="G10" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="H10" s="103" t="s">
+      <c r="H10" s="45" t="s">
         <v>161</v>
       </c>
       <c r="I10" s="8" t="s">
@@ -3034,7 +3147,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="30">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="57" t="s">
         <v>172</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -3060,7 +3173,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="89"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="23" t="s">
         <v>152</v>
       </c>
@@ -3087,7 +3200,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="89"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="23" t="s">
         <v>153</v>
       </c>
@@ -3112,7 +3225,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="89"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="23" t="s">
         <v>154</v>
       </c>
@@ -3137,7 +3250,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="89"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="24" t="s">
         <v>155</v>
       </c>
@@ -3164,8 +3277,8 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="89"/>
-      <c r="B16" s="100" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="56" t="s">
         <v>176</v>
       </c>
       <c r="C16" s="25" t="s">
@@ -3192,8 +3305,8 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="89"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="25" t="s">
         <v>5</v>
       </c>
@@ -3218,8 +3331,8 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="89"/>
-      <c r="B18" s="100"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="25" t="s">
         <v>5</v>
       </c>
@@ -3239,8 +3352,8 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="89"/>
-      <c r="B19" s="100"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="25" t="s">
         <v>5</v>
       </c>
@@ -3286,7 +3399,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="A1:XFD1048576"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3394,7 +3507,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="62" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -3407,7 +3520,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="51"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -3418,7 +3531,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="64" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3441,7 +3554,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="53"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -3713,15 +3826,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -3757,7 +3870,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="67" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -3783,7 +3896,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="56"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -3807,7 +3920,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -3885,42 +3998,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="54" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="54"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="66"/>
+      <c r="D2" s="78"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -3952,16 +4065,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="73" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="67" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -3981,12 +4094,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="62"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="68"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -4004,12 +4117,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="62"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -4019,7 +4132,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="63"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -4103,41 +4216,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="79" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="80" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="82"/>
+      <c r="C3" s="94"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -4164,14 +4277,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="75"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="30" t="s">
         <v>103</v>
       </c>
@@ -4195,11 +4308,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="83" t="s">
+      <c r="A5" s="74"/>
+      <c r="B5" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -4226,12 +4339,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="76" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
       <c r="E6" s="30" t="s">
         <v>109</v>
       </c>
@@ -4255,11 +4368,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="62"/>
-      <c r="B7" s="67" t="s">
+      <c r="A7" s="74"/>
+      <c r="B7" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="34" t="s">
         <v>114</v>
       </c>
@@ -4286,9 +4399,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="62"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="35" t="s">
         <v>120</v>
       </c>
@@ -4315,9 +4428,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="62"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="34" t="s">
         <v>121</v>
       </c>
@@ -4344,9 +4457,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="63"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="34" t="s">
         <v>122</v>
       </c>
@@ -4416,31 +4529,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="94" t="s">
+      <c r="D1" s="99"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="94" t="s">
+      <c r="G1" s="99"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="95"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="97" t="s">
+      <c r="J1" s="99"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="94" t="s">
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="96"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="100"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4761,26 +4874,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="94" t="s">
+      <c r="D1" s="99"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="95"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="94" t="s">
+      <c r="G1" s="99"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="95"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="97" t="s">
+      <c r="J1" s="99"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
add test in SBT
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F01C691-C4EB-480A-B7D8-3EA5CE8BA071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592F3F76-6BFA-48F6-A1DD-F1AB361CB067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="188">
   <si>
     <t>Role</t>
   </si>
@@ -606,6 +606,9 @@
   </si>
   <si>
     <t>Expected1</t>
+  </si>
+  <si>
+    <t>Scenario2:expected</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -2919,10 +2922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
-  <dimension ref="A3:I19"/>
+  <dimension ref="A3:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2936,9 +2939,12 @@
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" s="58" t="s">
         <v>1</v>
       </c>
@@ -2962,8 +2968,13 @@
       </c>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="61"/>
@@ -2981,8 +2992,17 @@
       <c r="I4" s="36" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="53" t="s">
         <v>28</v>
       </c>
@@ -3010,8 +3030,17 @@
       <c r="I5" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="53"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
@@ -3037,8 +3066,17 @@
       <c r="I6" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="53"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
@@ -3064,8 +3102,17 @@
       <c r="I7" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="40">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="53"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
@@ -3091,8 +3138,17 @@
       <c r="I8" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="53"/>
       <c r="B9" s="23" t="s">
         <v>179</v>
@@ -3118,8 +3174,17 @@
       <c r="I9" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="53"/>
       <c r="B10" s="43" t="s">
         <v>180</v>
@@ -3145,8 +3210,17 @@
       <c r="I10" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+      <c r="J10" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="K10" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
       <c r="A11" s="57" t="s">
         <v>172</v>
       </c>
@@ -3171,8 +3245,14 @@
       <c r="I11" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="K11" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="57"/>
       <c r="B12" s="23" t="s">
         <v>152</v>
@@ -3198,8 +3278,17 @@
       <c r="I12" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="57"/>
       <c r="B13" s="23" t="s">
         <v>153</v>
@@ -3223,8 +3312,15 @@
       <c r="I13" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="2"/>
+      <c r="K13" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="57"/>
       <c r="B14" s="23" t="s">
         <v>154</v>
@@ -3248,8 +3344,15 @@
       <c r="I14" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="2"/>
+      <c r="K14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="57"/>
       <c r="B15" s="24" t="s">
         <v>155</v>
@@ -3275,8 +3378,17 @@
       <c r="I15" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="57"/>
       <c r="B16" s="56" t="s">
         <v>176</v>
@@ -3303,8 +3415,18 @@
       <c r="I16" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="2" t="str">
+        <f>J16</f>
+        <v>V1.1</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="57"/>
       <c r="B17" s="56"/>
       <c r="C17" s="25" t="s">
@@ -3329,8 +3451,18 @@
       <c r="I17" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2" t="str">
+        <f t="shared" ref="K17:K19" si="1">J17</f>
+        <v>V2.1</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="57"/>
       <c r="B18" s="56"/>
       <c r="C18" s="25" t="s">
@@ -3350,8 +3482,13 @@
       <c r="I18" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="57"/>
       <c r="B19" s="56"/>
       <c r="C19" s="25" t="s">
@@ -3376,9 +3513,20 @@
       <c r="I19" s="8" t="s">
         <v>145</v>
       </c>
+      <c r="J19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" s="2" t="str">
+        <f t="shared" ref="K19:K21" si="2">J19</f>
+        <v>2021/4/30</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>145</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="J3:L3"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="B16:B19"/>

</xml_diff>

<commit_message>
use junitxml in Pester
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23167667-610B-4AD6-9FED-5BAE4E82AC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7CB82E-2925-4133-9FF8-C5BD08755AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="2" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
     <sheet name="SpecificationByTestcase" sheetId="9" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
-    <sheet name="StoryExample1" sheetId="8" r:id="rId7"/>
+    <sheet name="StoryExample1" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
     <sheet name="SBTSheet1" sheetId="7" r:id="rId8"/>
     <sheet name="SBTSheet2" sheetId="10" r:id="rId9"/>
     <sheet name="SBTSheet3" sheetId="11" r:id="rId10"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="190">
   <si>
     <t>Role</t>
   </si>
@@ -609,6 +609,12 @@
   </si>
   <si>
     <t>Scenario5:Expected@V0.2</t>
+  </si>
+  <si>
+    <t>Scenario6:TestResult@V0.2</t>
+  </si>
+  <si>
+    <t>SBTSheet2</t>
   </si>
 </sst>
 </file>
@@ -681,7 +687,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,6 +738,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -910,7 +928,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1180,6 +1198,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1644,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1658,12 +1689,13 @@
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45">
+    <row r="1" spans="1:11" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1694,8 +1726,11 @@
       <c r="J1" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="30">
+      <c r="K1" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1726,8 +1761,11 @@
       <c r="J2" s="7" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -1758,8 +1796,11 @@
       <c r="J3" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="30">
+      <c r="K3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -1790,16 +1831,19 @@
       <c r="J4" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23" t="s">
+      <c r="K4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="104"/>
+      <c r="B5" s="105" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="106" t="s">
         <v>175</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -1820,16 +1864,19 @@
       <c r="J5" s="7" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="22"/>
-      <c r="B6" s="43" t="s">
+      <c r="K5" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="104"/>
+      <c r="B6" s="107" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="106" t="s">
         <v>175</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -1850,8 +1897,11 @@
       <c r="J6" s="7" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="30">
+      <c r="K6" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -1882,8 +1932,11 @@
       <c r="J7" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="22">
         <v>5</v>
       </c>
@@ -1914,8 +1967,11 @@
       <c r="J8" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -1946,8 +2002,11 @@
       <c r="J9" s="7">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="30">
+      <c r="K9" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -1978,8 +2037,11 @@
       <c r="J10" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="30">
+      <c r="K10" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -2010,8 +2072,11 @@
       <c r="J11" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -2032,8 +2097,9 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" ht="30">
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" ht="30">
       <c r="A13" s="22">
         <v>10</v>
       </c>
@@ -2054,8 +2120,9 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="45">
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="46">
         <v>11</v>
       </c>
@@ -2086,8 +2153,11 @@
       <c r="J14" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="47"/>
       <c r="B15" s="20" t="s">
         <v>97</v>
@@ -2102,8 +2172,9 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="47"/>
       <c r="B16" s="20" t="s">
         <v>84</v>
@@ -2118,8 +2189,9 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="48"/>
       <c r="B17" s="21" t="s">
         <v>85</v>
@@ -2134,8 +2206,9 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" s="25">
         <v>12</v>
       </c>
@@ -2166,8 +2239,11 @@
       <c r="J18" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="30">
+      <c r="K18" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="25">
         <v>13</v>
       </c>
@@ -2183,23 +2259,26 @@
       <c r="E19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="108">
         <v>5</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="108">
         <v>5</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="108">
         <v>5</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="108">
         <v>5</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="108">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="108">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
         <v>14</v>
       </c>
@@ -2228,7 +2307,10 @@
         <v>4</v>
       </c>
       <c r="J20" s="7">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="K20" s="7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2667,7 +2749,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2698,9 +2780,7 @@
         <v>66</v>
       </c>
       <c r="J1" s="102"/>
-      <c r="K1" s="98" t="s">
-        <v>131</v>
-      </c>
+      <c r="K1" s="98"/>
       <c r="L1" s="99"/>
     </row>
     <row r="2" spans="1:12">
@@ -2734,12 +2814,8 @@
       <c r="J2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>143</v>
-      </c>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="22" t="s">
@@ -2776,13 +2852,8 @@
         <f>I3</f>
         <v>V1.4</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="L3" s="8" t="str">
-        <f>K3</f>
-        <v>V1.5</v>
-      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="22" t="s">
@@ -2819,13 +2890,8 @@
         <f t="shared" ref="J4:J6" si="3">I4</f>
         <v>V2.4</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L4" s="8" t="str">
-        <f t="shared" ref="L4" si="4">K4</f>
-        <v>V2.5</v>
-      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="38" t="s">
@@ -2880,13 +2946,8 @@
         <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="K6" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="L6" s="8">
-        <f t="shared" ref="L6" si="5">K6</f>
-        <v>5.4</v>
-      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
@@ -3543,11 +3604,320 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="91" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+    </row>
+    <row r="2" spans="1:11" ht="38.25" customHeight="1">
+      <c r="A2" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="94"/>
+      <c r="D3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1">
+      <c r="A4" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="51.75" customHeight="1">
+      <c r="A5" s="74"/>
+      <c r="B5" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="95"/>
+      <c r="D5" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="31">
+        <v>22</v>
+      </c>
+      <c r="G5" s="31">
+        <v>22</v>
+      </c>
+      <c r="H5" s="31">
+        <v>22</v>
+      </c>
+      <c r="I5" s="31">
+        <v>22</v>
+      </c>
+      <c r="J5" s="31">
+        <v>13</v>
+      </c>
+      <c r="K5" s="31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33.75" customHeight="1">
+      <c r="A6" s="74"/>
+      <c r="B6" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="31.5">
+      <c r="A7" s="74"/>
+      <c r="B7" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="80"/>
+      <c r="D7" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
+      <c r="A8" s="74"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="31.5">
+      <c r="A9" s="74"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="31">
+        <v>345</v>
+      </c>
+      <c r="G9" s="31">
+        <v>567</v>
+      </c>
+      <c r="H9" s="31">
+        <v>2100</v>
+      </c>
+      <c r="I9" s="31">
+        <v>452</v>
+      </c>
+      <c r="J9" s="31">
+        <v>643</v>
+      </c>
+      <c r="K9" s="31">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="31.5">
+      <c r="A10" s="75"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="33">
+        <v>0.45</v>
+      </c>
+      <c r="H10" s="33">
+        <v>0.65</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0.67</v>
+      </c>
+      <c r="J10" s="33">
+        <v>0.45</v>
+      </c>
+      <c r="K10" s="33">
+        <v>0.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B7:C10"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5657C2-106C-47C7-BF16-329C2F267F09}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3743,7 +4113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A494DA1E-3A4D-414E-886D-A717DFF21DE7}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -3957,7 +4327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3FD2D2-D808-401C-A638-EED224C6394A}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -4128,7 +4498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9F3738-1988-486F-BE99-D486460FE985}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -4343,321 +4713,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="91" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-    </row>
-    <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="97" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="92" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="73" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="85" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="74"/>
-      <c r="B5" s="95" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="31">
-        <v>22</v>
-      </c>
-      <c r="G5" s="31">
-        <v>22</v>
-      </c>
-      <c r="H5" s="31">
-        <v>22</v>
-      </c>
-      <c r="I5" s="31">
-        <v>22</v>
-      </c>
-      <c r="J5" s="31">
-        <v>13</v>
-      </c>
-      <c r="K5" s="31">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="74"/>
-      <c r="B6" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="K6" s="31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="74"/>
-      <c r="B7" s="79" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="J7" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="74"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="K8" s="31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="74"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="31">
-        <v>345</v>
-      </c>
-      <c r="G9" s="31">
-        <v>567</v>
-      </c>
-      <c r="H9" s="31">
-        <v>2100</v>
-      </c>
-      <c r="I9" s="31">
-        <v>452</v>
-      </c>
-      <c r="J9" s="31">
-        <v>643</v>
-      </c>
-      <c r="K9" s="31">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="75"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="33">
-        <v>0.45</v>
-      </c>
-      <c r="H10" s="33">
-        <v>0.65</v>
-      </c>
-      <c r="I10" s="33">
-        <v>0.67</v>
-      </c>
-      <c r="J10" s="33">
-        <v>0.45</v>
-      </c>
-      <c r="K10" s="33">
-        <v>0.34</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:C10"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
java let exception throw out
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,22 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D770229D-C8C7-4562-91B7-7333D9DDFE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAA2D2B-94E1-4A15-8963-2D7E89119919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="5130" windowWidth="21600" windowHeight="11385" tabRatio="738" activeTab="10" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="2" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
     <sheet name="SpecificationByTestcase" sheetId="9" r:id="rId2"/>
-    <sheet name="StoryExample1" sheetId="8" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
-    <sheet name="SBTSheet1" sheetId="7" r:id="rId8"/>
-    <sheet name="SBTSheet2" sheetId="10" r:id="rId9"/>
-    <sheet name="SBTSheet3" sheetId="11" r:id="rId10"/>
-    <sheet name="Expected1" sheetId="13" r:id="rId11"/>
+    <sheet name="Exceptions" sheetId="15" r:id="rId3"/>
+    <sheet name="Sheet7" sheetId="16" r:id="rId4"/>
+    <sheet name="StoryExample1" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId9"/>
+    <sheet name="SBTSheet1" sheetId="7" r:id="rId10"/>
+    <sheet name="SBTSheet2" sheetId="10" r:id="rId11"/>
+    <sheet name="SBTSheet3" sheetId="11" r:id="rId12"/>
+    <sheet name="Expected1" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet5" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="212">
   <si>
     <t>Role</t>
   </si>
@@ -615,6 +618,72 @@
   </si>
   <si>
     <t>SBTSheet2</t>
+  </si>
+  <si>
+    <t>Sunday isn't Friday</t>
+  </si>
+  <si>
+    <t>Cucumber Simple example</t>
+  </si>
+  <si>
+    <t>https://cucumber.io/docs/guides/10-minute-tutorial/</t>
+  </si>
+  <si>
+    <t>Feature: Is it Friday yet?</t>
+  </si>
+  <si>
+    <t>Everybody wants to know when it's Friday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Given a day</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>When I ask whether it's Dedicate weekday？</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Then I should be told</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Nope</t>
+  </si>
+  <si>
+    <t>DayofWeek</t>
+  </si>
+  <si>
+    <t>Wrong worksheet</t>
+  </si>
+  <si>
+    <t>Wrong File</t>
+  </si>
+  <si>
+    <t>wrongfile.xlsx</t>
+  </si>
+  <si>
+    <t>FileNotFoundException</t>
+  </si>
+  <si>
+    <t>WrongWorksheet</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>IOException</t>
+  </si>
+  <si>
+    <t>WrongWorksheet does not exist.</t>
   </si>
 </sst>
 </file>
@@ -687,7 +756,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -750,6 +819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -928,7 +1003,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1038,6 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1212,6 +1288,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1678,7 +1764,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1689,9 +1775,9 @@
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2123,19 +2209,19 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="45">
-      <c r="A14" s="51">
+      <c r="A14" s="52">
         <v>11</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="55" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="56" t="s">
         <v>86</v>
       </c>
       <c r="F14" s="7">
@@ -2158,15 +2244,15 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="52"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E15" s="56"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -2175,15 +2261,15 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="52"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="56"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -2192,15 +2278,15 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="53"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="54"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="57"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -2325,6 +2411,703 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="105"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="104" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="105"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="104" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="105"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="104" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="106"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="O2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>C3</f>
+        <v>V1.1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="str">
+        <f>F3</f>
+        <v>V1.2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="8" t="str">
+        <f>I3</f>
+        <v>V1.3</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="8" t="str">
+        <f>L3</f>
+        <v>V1.4</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="8" t="str">
+        <f>O3</f>
+        <v>V1.5</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f t="shared" ref="D4:D6" si="0">C4</f>
+        <v>V2.1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f t="shared" ref="G4:G6" si="1">F4</f>
+        <v>V2.2</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f t="shared" ref="J4:J6" si="2">I4</f>
+        <v>V2.3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f t="shared" ref="M4:M6" si="3">L4</f>
+        <v>V2.4</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="8" t="str">
+        <f t="shared" ref="P4" si="4">O4</f>
+        <v>V2.5</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="O6" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6" si="5">O6</f>
+        <v>5.4</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD4D131-69ED-4813-926B-7E95E2B369DB}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="105"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="104" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="105"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="104" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="105"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>C4</f>
+        <v>V1.1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f>F4</f>
+        <v>V1.2</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f>I4</f>
+        <v>V1.3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f>L4</f>
+        <v>V1.4</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="22"/>
+      <c r="B5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f t="shared" ref="D8:D10" si="0">C8</f>
+        <v>V2.1</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="8" t="str">
+        <f t="shared" ref="G8:G10" si="1">F8</f>
+        <v>V2.2</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="8" t="str">
+        <f t="shared" ref="J8:J10" si="2">I8</f>
+        <v>V2.3</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="8" t="str">
+        <f t="shared" ref="M8:M10" si="3">L8</f>
+        <v>V2.4</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+      <c r="L15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27202F44-224C-40C0-ACC3-02135A9560D7}">
   <dimension ref="A1:V11"/>
   <sheetViews>
@@ -2350,36 +3133,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="103" t="s">
+      <c r="F1" s="105"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="103" t="s">
+      <c r="I1" s="105"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="104"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="108" t="s">
+      <c r="L1" s="105"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="103" t="s">
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="104"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="103" t="s">
+      <c r="R1" s="105"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="104" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="104"/>
-      <c r="V1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="106"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2744,12 +3527,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFF208A-E752-404F-A219-18F91B0322F1}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2764,24 +3547,24 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="103" t="s">
+      <c r="D1" s="105"/>
+      <c r="E1" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="103" t="s">
+      <c r="F1" s="105"/>
+      <c r="G1" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="104"/>
-      <c r="I1" s="106" t="s">
+      <c r="H1" s="105"/>
+      <c r="I1" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="104"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="105"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -2981,12 +3764,99 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ACBBF6-9F77-42E6-ADBF-E42E08CDCCFD}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="51" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30">
+      <c r="A6" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{59B266E9-07BA-44FE-AEB7-9901B990F12E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
   <dimension ref="A3:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3006,41 +3876,41 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="66" t="s">
         <v>159</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="58" t="s">
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
@@ -3064,7 +3934,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="61" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -3102,7 +3972,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="60"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
@@ -3138,7 +4008,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="60"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
@@ -3174,7 +4044,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="60"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
@@ -3210,7 +4080,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="60"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="23" t="s">
         <v>179</v>
       </c>
@@ -3246,7 +4116,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="60"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="43" t="s">
         <v>180</v>
       </c>
@@ -3282,7 +4152,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="63" t="s">
         <v>172</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -3314,7 +4184,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="62"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="23" t="s">
         <v>152</v>
       </c>
@@ -3350,7 +4220,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="62"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="23" t="s">
         <v>153</v>
       </c>
@@ -3382,7 +4252,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="62"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="23" t="s">
         <v>154</v>
       </c>
@@ -3414,7 +4284,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="62"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="24" t="s">
         <v>155</v>
       </c>
@@ -3450,8 +4320,8 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="62"/>
-      <c r="B16" s="61" t="s">
+      <c r="A16" s="63"/>
+      <c r="B16" s="62" t="s">
         <v>176</v>
       </c>
       <c r="C16" s="25" t="s">
@@ -3488,8 +4358,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="62"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="25" t="s">
         <v>5</v>
       </c>
@@ -3524,8 +4394,8 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="62"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="62"/>
       <c r="C18" s="25" t="s">
         <v>5</v>
       </c>
@@ -3550,8 +4420,8 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="62"/>
-      <c r="B19" s="61"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="25" t="s">
         <v>5</v>
       </c>
@@ -3604,6 +4474,214 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4E5E2-8FAC-4516-9FEA-053724A7E1DD}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="109"/>
+      <c r="F1" s="104" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="105"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="112" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="113" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="113" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="112"/>
+      <c r="B4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="113" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="113" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
+      <c r="A5" s="112"/>
+      <c r="B5" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="110">
+        <v>2</v>
+      </c>
+      <c r="E5" s="113"/>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="G5" s="113"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="112"/>
+      <c r="B6" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="111" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="113"/>
+      <c r="F6" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="113"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DB7B63-E032-433E-B0E0-E6E5C56D92F2}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="104" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="105"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>A3</f>
+        <v>V1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>A4</f>
+        <v>V2.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="b">
+        <f>A6</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -3624,41 +4702,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="85"/>
+      <c r="C3" s="86"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -3685,14 +4763,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="30" t="s">
         <v>103</v>
       </c>
@@ -3716,11 +4794,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="86" t="s">
+      <c r="A5" s="81"/>
+      <c r="B5" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="86"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -3747,12 +4825,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="80"/>
-      <c r="B6" s="76" t="s">
+      <c r="A6" s="81"/>
+      <c r="B6" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
       <c r="E6" s="30" t="s">
         <v>109</v>
       </c>
@@ -3776,11 +4854,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="80"/>
-      <c r="B7" s="67" t="s">
+      <c r="A7" s="81"/>
+      <c r="B7" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="34" t="s">
         <v>114</v>
       </c>
@@ -3807,9 +4885,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="80"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="35" t="s">
         <v>120</v>
       </c>
@@ -3836,9 +4914,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="80"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="34" t="s">
         <v>121</v>
       </c>
@@ -3865,9 +4943,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="81"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="34" t="s">
         <v>122</v>
       </c>
@@ -3912,12 +4990,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5657C2-106C-47C7-BF16-329C2F267F09}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4025,7 +5103,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="90" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4038,7 +5116,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="90"/>
+      <c r="A8" s="91"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -4049,7 +5127,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="92" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -4072,7 +5150,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="92"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -4113,7 +5191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A494DA1E-3A4D-414E-886D-A717DFF21DE7}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -4327,7 +5405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3FD2D2-D808-401C-A638-EED224C6394A}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -4344,15 +5422,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -4388,7 +5466,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="95" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -4414,7 +5492,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="95"/>
+      <c r="C4" s="96"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -4438,7 +5516,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="96"/>
+      <c r="C5" s="97"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -4498,7 +5576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9F3738-1988-486F-BE99-D486460FE985}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -4516,42 +5594,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="93" t="s">
+      <c r="B1" s="100"/>
+      <c r="C1" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="93"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="102" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="102"/>
+      <c r="D2" s="103"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="102"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -4583,16 +5661,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="80" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="95" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -4612,12 +5690,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="80"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="95"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="96"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -4635,12 +5713,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="80"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="96"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="97"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -4650,7 +5728,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="81"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -4711,701 +5789,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
-  <dimension ref="A1:Q11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="B1" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="103" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="103" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="104"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="103" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="104"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="106" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="103" t="s">
-        <v>131</v>
-      </c>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="105"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="O2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" s="36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="8" t="str">
-        <f>C3</f>
-        <v>V1.1</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="8" t="str">
-        <f>F3</f>
-        <v>V1.2</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="8" t="str">
-        <f>I3</f>
-        <v>V1.3</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="8" t="str">
-        <f>L3</f>
-        <v>V1.4</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="P3" s="8" t="str">
-        <f>O3</f>
-        <v>V1.5</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="8" t="str">
-        <f t="shared" ref="D4:D6" si="0">C4</f>
-        <v>V2.1</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="8" t="str">
-        <f t="shared" ref="G4:G6" si="1">F4</f>
-        <v>V2.2</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="8" t="str">
-        <f t="shared" ref="J4:J6" si="2">I4</f>
-        <v>V2.3</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="8" t="str">
-        <f t="shared" ref="M4:M6" si="3">L4</f>
-        <v>V2.4</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="8" t="str">
-        <f t="shared" ref="P4" si="4">O4</f>
-        <v>V2.5</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>2021/4/30</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I6" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="8" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L6" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M6" s="8">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="O6" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="P6" s="8">
-        <f t="shared" ref="P6" si="5">O6</f>
-        <v>5.4</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" t="s">
-        <v>88</v>
-      </c>
-      <c r="L11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="O1:Q1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD4D131-69ED-4813-926B-7E95E2B369DB}">
-  <dimension ref="A1:N15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="B1" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="103" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="104"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="103" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="104"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="103" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="104"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="106" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8" t="str">
-        <f>C4</f>
-        <v>V1.1</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="8" t="str">
-        <f>F4</f>
-        <v>V1.2</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="8" t="str">
-        <f>I4</f>
-        <v>V1.3</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="8" t="str">
-        <f>L4</f>
-        <v>V1.4</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="22"/>
-      <c r="B5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="8" t="str">
-        <f t="shared" ref="D8:D10" si="0">C8</f>
-        <v>V2.1</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="8" t="str">
-        <f t="shared" ref="G8:G10" si="1">F8</f>
-        <v>V2.2</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="8" t="str">
-        <f t="shared" ref="J8:J10" si="2">I8</f>
-        <v>V2.3</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="8" t="str">
-        <f t="shared" ref="M8:M10" si="3">L8</f>
-        <v>V2.4</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>2021/4/30</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F10" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" s="8" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="L10" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M10" s="8">
-        <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" t="s">
-        <v>88</v>
-      </c>
-      <c r="L15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add sub-step in SpecificationByExample
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C93191-5BA5-43A4-8A67-046EE64DC2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CDB11C-5085-4041-9F68-9B51B11CF285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="3" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="215">
   <si>
     <t>Role</t>
   </si>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t>WrongExcelSettings</t>
+  </si>
+  <si>
+    <t>Edit requirements sheet in excel, just as this excel sheet, select this sheet</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1012,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1106,7 +1109,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1303,6 +1305,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1767,215 +1787,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45">
+    <row r="1" spans="1:12" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30">
+    <row r="2" spans="1:12">
       <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="113" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>11</v>
+      <c r="F2" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>160</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>149</v>
+      <c r="B3" s="114"/>
+      <c r="C3" s="23" t="s">
+        <v>151</v>
       </c>
       <c r="D3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
-        <v>2</v>
-      </c>
-      <c r="I3" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" s="8">
-        <v>2</v>
-      </c>
-      <c r="K3" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30">
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="22">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="114"/>
+      <c r="C4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2</v>
+      </c>
+      <c r="J4" s="8">
+        <v>3</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="114"/>
+      <c r="C5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="D5" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="E5" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="114"/>
+      <c r="C6" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="E6" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>184</v>
@@ -1992,424 +2024,481 @@
       <c r="K6" s="7" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30">
+      <c r="L6" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="22">
-        <v>4</v>
-      </c>
-      <c r="B7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="115"/>
+      <c r="C7" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="116" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="D8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="E8" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="22">
+    <row r="9" spans="1:12">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="117"/>
+      <c r="C9" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="E9" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="22">
+        <v>9</v>
+      </c>
+      <c r="B10" s="117"/>
+      <c r="C10" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="22">
-        <v>6</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="25" t="s">
+      <c r="F10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L10" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="117"/>
+      <c r="C11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E11" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G9" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H9" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I9" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J9" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K9" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="30">
-      <c r="A10" s="22">
-        <v>7</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="F11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" s="22">
+        <v>11</v>
+      </c>
+      <c r="B12" s="117"/>
+      <c r="C12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="E12" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30">
-      <c r="A11" s="22">
-        <v>8</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="25" t="s">
+      <c r="F12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="22">
+        <v>12</v>
+      </c>
+      <c r="B13" s="117"/>
+      <c r="C13" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="E13" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="22">
-        <v>9</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" ht="30">
-      <c r="A13" s="22">
-        <v>10</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="45">
-      <c r="A14" s="55">
-        <v>11</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="22">
+        <v>13</v>
+      </c>
+      <c r="B14" s="117"/>
+      <c r="C14" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" s="54">
+        <v>14</v>
+      </c>
+      <c r="B15" s="117"/>
+      <c r="C15" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="D15" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="E15" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="F15" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G15" s="7">
         <v>3</v>
       </c>
-      <c r="G14" s="7">
+      <c r="H15" s="7">
         <v>3</v>
       </c>
-      <c r="H14" s="7">
+      <c r="I15" s="7">
         <v>3</v>
       </c>
-      <c r="I14" s="7">
+      <c r="J15" s="7">
         <v>3</v>
       </c>
-      <c r="J14" s="7">
+      <c r="K15" s="7">
         <v>3</v>
       </c>
-      <c r="K14" s="7">
+      <c r="L15" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="56"/>
-      <c r="B15" s="20" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" s="55"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="25" t="s">
+      <c r="D16" s="57"/>
+      <c r="E16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="56"/>
-      <c r="B16" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="59"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="57"/>
-      <c r="B17" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="25" t="s">
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="55"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="59"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="1:11" ht="30">
-      <c r="A18" s="25">
-        <v>12</v>
-      </c>
-      <c r="B18" s="26" t="s">
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="56"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="57"/>
+      <c r="E18" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="60"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="1:12" ht="30">
+      <c r="A19" s="25">
+        <v>15</v>
+      </c>
+      <c r="B19" s="117"/>
+      <c r="C19" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="D19" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="E19" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30">
-      <c r="A19" s="25">
+    <row r="20" spans="1:12" ht="30">
+      <c r="A20" s="25">
+        <v>16</v>
+      </c>
+      <c r="B20" s="117"/>
+      <c r="C20" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="49">
+        <v>5</v>
+      </c>
+      <c r="H20" s="49">
+        <v>5</v>
+      </c>
+      <c r="I20" s="49">
+        <v>5</v>
+      </c>
+      <c r="J20" s="49">
+        <v>5</v>
+      </c>
+      <c r="K20" s="49">
+        <v>9</v>
+      </c>
+      <c r="L20" s="49">
         <v>13</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="25" t="s">
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="118"/>
+      <c r="C21" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="E21" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="50">
-        <v>5</v>
-      </c>
-      <c r="G19" s="50">
-        <v>5</v>
-      </c>
-      <c r="H19" s="50">
-        <v>5</v>
-      </c>
-      <c r="I19" s="50">
-        <v>5</v>
-      </c>
-      <c r="J19" s="50">
-        <v>9</v>
-      </c>
-      <c r="K19" s="50">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="2">
-        <v>14</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F20" s="7">
+      <c r="G21" s="7">
         <v>4</v>
       </c>
-      <c r="G20" s="7">
+      <c r="H21" s="7">
         <v>4</v>
       </c>
-      <c r="H20" s="7">
+      <c r="I21" s="7">
         <v>4</v>
       </c>
-      <c r="I20" s="7">
+      <c r="J21" s="7">
         <v>4</v>
       </c>
-      <c r="J20" s="7">
+      <c r="K21" s="7">
         <v>4</v>
       </c>
-      <c r="K20" s="7">
+      <c r="L21" s="7">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="E14:E17"/>
+  <mergeCells count="5">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2441,31 +2530,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="72" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="72" t="s">
+      <c r="G1" s="72"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="112" t="s">
+      <c r="J1" s="72"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="72" t="s">
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="111"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="110"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -2786,26 +2875,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="72" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="73"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="72" t="s">
+      <c r="G1" s="72"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="112" t="s">
+      <c r="J1" s="72"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3139,36 +3228,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="72" t="s">
+      <c r="F1" s="72"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="73"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="72" t="s">
+      <c r="I1" s="72"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="73"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="74" t="s">
+      <c r="L1" s="72"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="72" t="s">
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="73"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="72" t="s">
+      <c r="R1" s="72"/>
+      <c r="S1" s="110"/>
+      <c r="T1" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="111"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="110"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -3553,24 +3642,24 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="72" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="72" t="s">
+      <c r="F1" s="72"/>
+      <c r="G1" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="112" t="s">
+      <c r="H1" s="72"/>
+      <c r="I1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="73"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="72"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -3795,7 +3884,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3862,7 +3951,7 @@
   <dimension ref="A3:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3882,41 +3971,41 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="68" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="68" t="s">
         <v>159</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="62" t="s">
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
@@ -3940,7 +4029,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="63" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -3978,7 +4067,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="64"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
@@ -4014,7 +4103,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="64"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
@@ -4031,7 +4120,7 @@
         <v>26</v>
       </c>
       <c r="G7" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>40</v>
@@ -4040,7 +4129,7 @@
         <v>145</v>
       </c>
       <c r="J7" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>186</v>
@@ -4050,7 +4139,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="64"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
@@ -4086,7 +4175,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="64"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="23" t="s">
         <v>179</v>
       </c>
@@ -4122,7 +4211,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="64"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="43" t="s">
         <v>180</v>
       </c>
@@ -4158,7 +4247,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="65" t="s">
         <v>172</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -4190,7 +4279,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="66"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="23" t="s">
         <v>152</v>
       </c>
@@ -4226,7 +4315,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="66"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="23" t="s">
         <v>153</v>
       </c>
@@ -4258,7 +4347,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="66"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="23" t="s">
         <v>154</v>
       </c>
@@ -4290,7 +4379,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="66"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="24" t="s">
         <v>155</v>
       </c>
@@ -4326,8 +4415,8 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="66"/>
-      <c r="B16" s="65" t="s">
+      <c r="A16" s="65"/>
+      <c r="B16" s="64" t="s">
         <v>176</v>
       </c>
       <c r="C16" s="25" t="s">
@@ -4364,8 +4453,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="66"/>
-      <c r="B17" s="65"/>
+      <c r="A17" s="65"/>
+      <c r="B17" s="64"/>
       <c r="C17" s="25" t="s">
         <v>5</v>
       </c>
@@ -4400,8 +4489,8 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="66"/>
-      <c r="B18" s="65"/>
+      <c r="A18" s="65"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="25" t="s">
         <v>5</v>
       </c>
@@ -4426,8 +4515,8 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="66"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="25" t="s">
         <v>5</v>
       </c>
@@ -4504,14 +4593,14 @@
       <c r="C1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="72" t="s">
+      <c r="E1" s="73"/>
+      <c r="F1" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="73"/>
+      <c r="G1" s="72"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
@@ -4537,7 +4626,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="70" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -4546,21 +4635,21 @@
       <c r="C3" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="53" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="71"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
@@ -4570,49 +4659,49 @@
       <c r="D4" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="53" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="71"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="51">
         <v>2</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="52">
+      <c r="E5" s="53"/>
+      <c r="F5" s="51">
         <v>2</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="71"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="54"/>
-      <c r="F6" s="52" t="s">
+      <c r="E6" s="53"/>
+      <c r="F6" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4628,7 +4717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DB7B63-E032-433E-B0E0-E6E5C56D92F2}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -4647,10 +4736,10 @@
       <c r="C1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="71" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="73"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
@@ -4670,7 +4759,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="70" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -4679,49 +4768,49 @@
       <c r="C3" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="54"/>
+      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="71"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="71"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="51">
         <v>1</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="53"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="71"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="54"/>
+      <c r="E6" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4753,41 +4842,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="90" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="91" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="93"/>
+      <c r="C3" s="92"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -4814,14 +4903,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="30" t="s">
         <v>103</v>
       </c>
@@ -4845,11 +4934,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="94" t="s">
+      <c r="A5" s="87"/>
+      <c r="B5" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="94"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -4876,12 +4965,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="88"/>
-      <c r="B6" s="84" t="s">
+      <c r="A6" s="87"/>
+      <c r="B6" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="86"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="85"/>
       <c r="E6" s="30" t="s">
         <v>109</v>
       </c>
@@ -4905,11 +4994,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="88"/>
-      <c r="B7" s="75" t="s">
+      <c r="A7" s="87"/>
+      <c r="B7" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="76"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="34" t="s">
         <v>114</v>
       </c>
@@ -4936,9 +5025,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="88"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="78"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="35" t="s">
         <v>120</v>
       </c>
@@ -4965,9 +5054,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="88"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="78"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="34" t="s">
         <v>121</v>
       </c>
@@ -4994,9 +5083,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="89"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="80"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="34" t="s">
         <v>122</v>
       </c>
@@ -5154,7 +5243,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="96" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -5167,7 +5256,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="98"/>
+      <c r="A8" s="97"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -5178,7 +5267,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="98" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5201,7 +5290,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="100"/>
+      <c r="A10" s="99"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -5473,15 +5562,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -5517,7 +5606,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="101" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -5543,7 +5632,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="102"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -5567,7 +5656,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="104"/>
+      <c r="C5" s="103"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -5645,42 +5734,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="101" t="s">
+      <c r="B1" s="106"/>
+      <c r="C1" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="101"/>
+      <c r="D1" s="100"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="105" t="s">
+      <c r="F1" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="110" t="s">
+      <c r="B2" s="106"/>
+      <c r="C2" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="110"/>
+      <c r="D2" s="109"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="109"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="108"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -5712,16 +5801,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="86" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="101" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -5741,12 +5830,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="88"/>
+      <c r="A5" s="87"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="103"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="102"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -5764,12 +5853,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="88"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="104"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="103"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -5779,7 +5868,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="89"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
cover SBT existing examples
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E105856\ExcelBDD\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084ECCA-793B-42C9-8492-1A84158FA55B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCB86C6-70A1-4D6A-8FE5-CD2BBA117FCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="2" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -1156,6 +1156,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1195,6 +1213,27 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1222,9 +1261,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1350,42 +1386,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1917,7 +1917,7 @@
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="67" t="s">
         <v>211</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -1958,7 +1958,7 @@
       <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
+      <c r="B3" s="68"/>
       <c r="C3" s="22" t="s">
         <v>150</v>
       </c>
@@ -1997,7 +1997,7 @@
       <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="22" t="s">
         <v>25</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="62"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="22" t="s">
         <v>27</v>
       </c>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="21"/>
-      <c r="B6" s="62"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="25" t="s">
         <v>89</v>
       </c>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="21"/>
-      <c r="B7" s="62"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="25" t="s">
         <v>216</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="A8" s="21">
         <v>5</v>
       </c>
-      <c r="B8" s="62"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="45" t="s">
         <v>178</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="A9" s="21">
         <v>6</v>
       </c>
-      <c r="B9" s="63"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="47" t="s">
         <v>179</v>
       </c>
@@ -2213,7 +2213,7 @@
       <c r="A10" s="21">
         <v>7</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="70" t="s">
         <v>171</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -2254,7 +2254,7 @@
       <c r="A11" s="21">
         <v>8</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="22" t="s">
         <v>31</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="A12" s="21">
         <v>9</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="22" t="s">
         <v>34</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="A13" s="21">
         <v>10</v>
       </c>
-      <c r="B13" s="65"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="23" t="s">
         <v>68</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="A14" s="21">
         <v>11</v>
       </c>
-      <c r="B14" s="65"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="23" t="s">
         <v>69</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="A15" s="21">
         <v>12</v>
       </c>
-      <c r="B15" s="65"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="23" t="s">
         <v>66</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="A16" s="21">
         <v>13</v>
       </c>
-      <c r="B16" s="65"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="22" t="s">
         <v>81</v>
       </c>
@@ -2457,20 +2457,20 @@
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" ht="28.8">
-      <c r="A17" s="54">
+      <c r="A17" s="60">
         <v>14</v>
       </c>
-      <c r="B17" s="65"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="63" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="64" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="7">
@@ -2496,16 +2496,16 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="55"/>
-      <c r="B18" s="65"/>
+      <c r="A18" s="61"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="57"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F18" s="59"/>
+      <c r="F18" s="65"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -2515,16 +2515,16 @@
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="55"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="57"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F19" s="59"/>
+      <c r="F19" s="65"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2534,16 +2534,16 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="56"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="57"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F20" s="60"/>
+      <c r="F20" s="66"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2556,7 +2556,7 @@
       <c r="A21" s="24">
         <v>16</v>
       </c>
-      <c r="B21" s="65"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="25" t="s">
         <v>36</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="B22" s="66"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="41" t="s">
         <v>163</v>
       </c>
@@ -2662,42 +2662,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="106" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="106"/>
+      <c r="D1" s="118"/>
       <c r="E1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="110" t="s">
+      <c r="F1" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="115" t="s">
+      <c r="B2" s="124"/>
+      <c r="C2" s="127" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="115"/>
+      <c r="D2" s="127"/>
       <c r="E2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="114"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="126"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -2729,16 +2729,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.900000000000006" customHeight="1">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="104" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="119" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2758,12 +2758,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.900000000000006" customHeight="1">
-      <c r="A5" s="93"/>
+      <c r="A5" s="105"/>
       <c r="B5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="108"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="120"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2781,12 +2781,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.900000000000006" customHeight="1">
-      <c r="A6" s="93"/>
+      <c r="A6" s="105"/>
       <c r="B6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="94"/>
-      <c r="D6" s="109"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="121"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2796,7 +2796,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="94"/>
+      <c r="A7" s="106"/>
       <c r="B7" s="9" t="s">
         <v>60</v>
       </c>
@@ -2885,31 +2885,31 @@
       <c r="B1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="77" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="77" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="117" t="s">
+      <c r="J1" s="90"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="77" t="s">
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="116"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="128"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -3231,26 +3231,26 @@
       <c r="B1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="77" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="77" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="117" t="s">
+      <c r="J1" s="90"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3585,36 +3585,36 @@
       <c r="D1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="78"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="77" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="78"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="77" t="s">
+      <c r="I1" s="90"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="78"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="79" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="77" t="s">
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="R1" s="78"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="77" t="s">
+      <c r="R1" s="90"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="U1" s="78"/>
-      <c r="V1" s="116"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="128"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -4000,24 +4000,24 @@
       <c r="B1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="77" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="78"/>
-      <c r="G1" s="77" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="117" t="s">
+      <c r="H1" s="90"/>
+      <c r="I1" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="118"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="78"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="90"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -4309,7 +4309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93BB7E4-E9BF-490F-8356-65B5D0024489}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -4374,7 +4374,7 @@
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="67" t="s">
         <v>211</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -4386,7 +4386,7 @@
       <c r="E2" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="127" t="s">
+      <c r="F2" s="59" t="s">
         <v>147</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -4415,7 +4415,7 @@
       <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
+      <c r="B3" s="68"/>
       <c r="C3" s="22" t="s">
         <v>150</v>
       </c>
@@ -4425,7 +4425,7 @@
       <c r="E3" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F3" s="127" t="s">
+      <c r="F3" s="59" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -4454,7 +4454,7 @@
       <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="25" t="s">
         <v>89</v>
       </c>
@@ -4487,7 +4487,7 @@
       <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="63"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="25" t="s">
         <v>216</v>
       </c>
@@ -4514,10 +4514,10 @@
       <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="54" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="24" t="s">
@@ -4526,7 +4526,7 @@
       <c r="E6" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="127" t="s">
+      <c r="F6" s="59" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -4555,8 +4555,8 @@
       <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="119" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="54" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -4565,7 +4565,7 @@
       <c r="E7" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="127" t="s">
+      <c r="F7" s="59" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -4594,8 +4594,8 @@
       <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="119" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="54" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="24" t="s">
@@ -4604,7 +4604,7 @@
       <c r="E8" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F8" s="127" t="s">
+      <c r="F8" s="59" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="7">
@@ -4633,8 +4633,8 @@
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="120" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="55" t="s">
         <v>68</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -4643,7 +4643,7 @@
       <c r="E9" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F9" s="127" t="s">
+      <c r="F9" s="59" t="s">
         <v>70</v>
       </c>
       <c r="G9" s="7" t="s">
@@ -4672,8 +4672,8 @@
       <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="120" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="55" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -4682,7 +4682,7 @@
       <c r="E10" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="127" t="s">
+      <c r="F10" s="59" t="s">
         <v>67</v>
       </c>
       <c r="G10" s="7" t="s">
@@ -4711,8 +4711,8 @@
       <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="120" t="s">
+      <c r="B11" s="73"/>
+      <c r="C11" s="55" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="24" t="s">
@@ -4721,7 +4721,7 @@
       <c r="E11" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F11" s="127" t="s">
+      <c r="F11" s="59" t="s">
         <v>35</v>
       </c>
       <c r="G11" s="7"/>
@@ -4736,8 +4736,8 @@
       <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="119" t="s">
+      <c r="B12" s="73"/>
+      <c r="C12" s="54" t="s">
         <v>81</v>
       </c>
       <c r="D12" s="24" t="s">
@@ -4746,7 +4746,7 @@
       <c r="E12" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F12" s="127" t="s">
+      <c r="F12" s="59" t="s">
         <v>82</v>
       </c>
       <c r="G12" s="7"/>
@@ -4758,20 +4758,20 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" ht="28.8">
-      <c r="A13" s="54">
+      <c r="A13" s="60">
         <v>12</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="119" t="s">
+      <c r="B13" s="73"/>
+      <c r="C13" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="128" t="s">
+      <c r="E13" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="F13" s="124" t="s">
+      <c r="F13" s="74" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="7">
@@ -4797,14 +4797,14 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="55"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="121" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="125"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="75"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -4814,14 +4814,14 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="55"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="121" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="57"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="125"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="75"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -4831,14 +4831,14 @@
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="56"/>
-      <c r="B16" s="76"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="126"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="76"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -4851,8 +4851,8 @@
       <c r="A17" s="24">
         <v>13</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="122" t="s">
+      <c r="B17" s="73"/>
+      <c r="C17" s="57" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="24" t="s">
@@ -4861,7 +4861,7 @@
       <c r="E17" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F17" s="127" t="s">
+      <c r="F17" s="59" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="7">
@@ -4890,8 +4890,8 @@
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="123" t="s">
+      <c r="B18" s="73"/>
+      <c r="C18" s="58" t="s">
         <v>163</v>
       </c>
       <c r="D18" s="24" t="s">
@@ -4900,7 +4900,7 @@
       <c r="E18" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F18" s="127" t="s">
+      <c r="F18" s="59" t="s">
         <v>164</v>
       </c>
       <c r="G18" s="7">
@@ -4943,8 +4943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
   <dimension ref="A3:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4959,46 +4959,46 @@
     <col min="8" max="8" width="16.5546875" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
     <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="87" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="87" t="s">
         <v>158</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="67" t="s">
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="80" t="s">
         <v>185</v>
       </c>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
+      <c r="A4" s="86"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
       <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
@@ -5022,7 +5022,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="82" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -5060,7 +5060,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="69"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="22" t="s">
         <v>150</v>
       </c>
@@ -5096,7 +5096,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="69"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
@@ -5132,7 +5132,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="69"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="22" t="s">
         <v>27</v>
       </c>
@@ -5168,7 +5168,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="69"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="22" t="s">
         <v>178</v>
       </c>
@@ -5204,7 +5204,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="69"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="42" t="s">
         <v>179</v>
       </c>
@@ -5240,7 +5240,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="84" t="s">
         <v>171</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -5272,7 +5272,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="71"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="22" t="s">
         <v>151</v>
       </c>
@@ -5308,7 +5308,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="71"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="22" t="s">
         <v>152</v>
       </c>
@@ -5340,7 +5340,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="71"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="22" t="s">
         <v>153</v>
       </c>
@@ -5372,7 +5372,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="71"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="23" t="s">
         <v>154</v>
       </c>
@@ -5408,8 +5408,8 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="71"/>
-      <c r="B16" s="70" t="s">
+      <c r="A16" s="84"/>
+      <c r="B16" s="83" t="s">
         <v>175</v>
       </c>
       <c r="C16" s="24" t="s">
@@ -5446,8 +5446,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="71"/>
-      <c r="B17" s="70"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="24" t="s">
         <v>5</v>
       </c>
@@ -5482,8 +5482,8 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="71"/>
-      <c r="B18" s="70"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="24" t="s">
         <v>5</v>
       </c>
@@ -5508,8 +5508,8 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="71"/>
-      <c r="B19" s="70"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="24" t="s">
         <v>5</v>
       </c>
@@ -5587,14 +5587,14 @@
       <c r="C1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="77" t="s">
+      <c r="E1" s="91"/>
+      <c r="F1" s="89" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="78"/>
+      <c r="G1" s="90"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
@@ -5620,7 +5620,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="73" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -5643,7 +5643,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="76"/>
+      <c r="A4" s="73"/>
       <c r="B4" s="22" t="s">
         <v>150</v>
       </c>
@@ -5664,7 +5664,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="76"/>
+      <c r="A5" s="73"/>
       <c r="B5" s="22" t="s">
         <v>25</v>
       </c>
@@ -5681,7 +5681,7 @@
       <c r="G5" s="52"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="76"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
@@ -5733,14 +5733,14 @@
       <c r="C1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="89" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="77" t="s">
+      <c r="E1" s="90"/>
+      <c r="F1" s="89" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="78"/>
+      <c r="G1" s="90"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
@@ -5766,7 +5766,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="73" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -5785,7 +5785,7 @@
       <c r="G3" s="52"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="76"/>
+      <c r="A4" s="73"/>
       <c r="B4" s="22" t="s">
         <v>150</v>
       </c>
@@ -5802,7 +5802,7 @@
       <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="76"/>
+      <c r="A5" s="73"/>
       <c r="B5" s="22" t="s">
         <v>25</v>
       </c>
@@ -5823,7 +5823,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="76"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
@@ -5875,41 +5875,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="95" t="s">
+      <c r="B1" s="112"/>
+      <c r="C1" s="107" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="96" t="s">
+      <c r="B2" s="113"/>
+      <c r="C2" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="98"/>
+      <c r="C3" s="110"/>
       <c r="D3" s="13" t="s">
         <v>110</v>
       </c>
@@ -5936,14 +5936,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="88"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="100"/>
       <c r="E4" s="29" t="s">
         <v>102</v>
       </c>
@@ -5967,11 +5967,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="93"/>
-      <c r="B5" s="99" t="s">
+      <c r="A5" s="105"/>
+      <c r="B5" s="111" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="99"/>
+      <c r="C5" s="111"/>
       <c r="D5" s="33" t="s">
         <v>112</v>
       </c>
@@ -5998,12 +5998,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="93"/>
-      <c r="B6" s="89" t="s">
+      <c r="A6" s="105"/>
+      <c r="B6" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="103"/>
       <c r="E6" s="29" t="s">
         <v>108</v>
       </c>
@@ -6027,11 +6027,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.2">
-      <c r="A7" s="93"/>
-      <c r="B7" s="80" t="s">
+      <c r="A7" s="105"/>
+      <c r="B7" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="81"/>
+      <c r="C7" s="93"/>
       <c r="D7" s="33" t="s">
         <v>113</v>
       </c>
@@ -6058,9 +6058,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="28.8">
-      <c r="A8" s="93"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
+      <c r="A8" s="105"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="34" t="s">
         <v>119</v>
       </c>
@@ -6087,9 +6087,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="95"/>
       <c r="D9" s="33" t="s">
         <v>120</v>
       </c>
@@ -6116,9 +6116,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.2">
-      <c r="A10" s="94"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
+      <c r="A10" s="106"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="33" t="s">
         <v>121</v>
       </c>
@@ -6276,7 +6276,7 @@
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="114" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -6289,7 +6289,7 @@
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="103"/>
+      <c r="A8" s="115"/>
       <c r="B8" s="4" t="s">
         <v>82</v>
       </c>
@@ -6300,7 +6300,7 @@
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="116" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -6323,7 +6323,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="105"/>
+      <c r="A10" s="117"/>
       <c r="B10" s="15" t="s">
         <v>82</v>
       </c>
@@ -6596,15 +6596,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -6640,7 +6640,7 @@
       <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="119" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -6666,7 +6666,7 @@
       <c r="B4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="108"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -6690,7 +6690,7 @@
       <c r="B5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="109"/>
+      <c r="C5" s="121"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
implement SmartBDD in Java
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123D3097-2B9A-41BD-9B97-52ABDDB2F35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581B29C8-FB16-4189-9239-55DD2B1BB22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="227">
   <si>
     <t>Role</t>
   </si>
@@ -1862,7 +1862,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4049,7 +4049,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4371,10 +4371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93BB7E4-E9BF-490F-8356-65B5D0024489}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4391,9 +4391,10 @@
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45">
+    <row r="1" spans="1:14" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -4433,8 +4434,11 @@
       <c r="M1" s="6" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1">
+      <c r="N1" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" customHeight="1">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -4474,8 +4478,11 @@
       <c r="M2" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -4513,8 +4520,11 @@
       <c r="M3" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="30">
+      <c r="N3" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -4546,8 +4556,11 @@
         <v>90</v>
       </c>
       <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -4573,8 +4586,9 @@
       <c r="M5" s="7" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="30">
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" ht="30">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -4614,8 +4628,11 @@
       <c r="M6" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -4653,8 +4670,11 @@
       <c r="M7" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -4692,8 +4712,11 @@
       <c r="M8" s="7">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="30">
+      <c r="N8" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -4731,8 +4754,11 @@
       <c r="M9" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="30">
+      <c r="N9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -4770,8 +4796,11 @@
       <c r="M10" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -4795,8 +4824,9 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="1:13" ht="30">
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="30">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -4820,8 +4850,9 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="1:13" ht="45">
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" ht="45">
       <c r="A13" s="60">
         <v>12</v>
       </c>
@@ -4859,8 +4890,11 @@
       <c r="M13" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="61"/>
       <c r="B14" s="73"/>
       <c r="C14" s="56" t="s">
@@ -4876,8 +4910,9 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="61"/>
       <c r="B15" s="73"/>
       <c r="C15" s="56" t="s">
@@ -4893,8 +4928,9 @@
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="62"/>
       <c r="B16" s="73"/>
       <c r="C16" s="20" t="s">
@@ -4910,8 +4946,9 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="1:13" ht="30">
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" ht="30">
       <c r="A17" s="24">
         <v>13</v>
       </c>
@@ -4949,8 +4986,11 @@
       <c r="M17" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -4986,6 +5026,9 @@
         <v>5</v>
       </c>
       <c r="M18" s="7">
+        <v>4</v>
+      </c>
+      <c r="N18" s="7">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add IOException on getExcelBDDStartPath
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4341107E-C492-41C8-978B-22F7D7E2F648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A4A07F-E41F-45D7-A6E9-EC2683FF2EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -680,9 +680,6 @@
     <t>IOException</t>
   </si>
   <si>
-    <t>WrongWorksheet does not exist.</t>
-  </si>
-  <si>
     <t>Edit requirements sheet in excel, just as this excel sheet, select this sheet</t>
   </si>
   <si>
@@ -732,6 +729,9 @@
   </si>
   <si>
     <t>notmatched</t>
+  </si>
+  <si>
+    <t>WrongWorksheet sheet does not exist.</t>
   </si>
 </sst>
 </file>
@@ -1924,10 +1924,10 @@
         <v>187</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1935,7 +1935,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>149</v>
@@ -2142,16 +2142,16 @@
       <c r="A7" s="21"/>
       <c r="B7" s="68"/>
       <c r="C7" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>148</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -2160,7 +2160,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N7" s="7"/>
     </row>
@@ -2325,13 +2325,13 @@
         <v>17</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -2367,13 +2367,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M12" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30">
@@ -3388,7 +3388,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D4" s="8" t="str">
         <f>C4</f>
@@ -3582,10 +3582,10 @@
         <v>144</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>144</v>
@@ -4377,7 +4377,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4414,7 +4414,7 @@
         <v>172</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>39</v>
@@ -4429,16 +4429,16 @@
         <v>53</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>223</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1">
@@ -4446,7 +4446,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>149</v>
@@ -4455,7 +4455,7 @@
         <v>148</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" s="59" t="s">
         <v>147</v>
@@ -4497,7 +4497,7 @@
         <v>148</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>6</v>
@@ -4539,7 +4539,7 @@
         <v>148</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="53" t="s">
         <v>95</v>
@@ -4569,16 +4569,16 @@
       </c>
       <c r="B5" s="69"/>
       <c r="C5" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>148</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4586,10 +4586,10 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N5" s="7"/>
     </row>
@@ -4607,7 +4607,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F6" s="59" t="s">
         <v>38</v>
@@ -4649,7 +4649,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F7" s="59" t="s">
         <v>32</v>
@@ -4676,7 +4676,7 @@
         <v>17</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -4691,7 +4691,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F8" s="59" t="s">
         <v>33</v>
@@ -4718,7 +4718,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30">
@@ -4733,7 +4733,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F9" s="59" t="s">
         <v>70</v>
@@ -4775,7 +4775,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F10" s="59" t="s">
         <v>67</v>
@@ -4817,7 +4817,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F11" s="59" t="s">
         <v>35</v>
@@ -4843,7 +4843,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F12" s="59" t="s">
         <v>82</v>
@@ -4869,7 +4869,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F13" s="74" t="s">
         <v>85</v>
@@ -4903,7 +4903,7 @@
       <c r="A14" s="61"/>
       <c r="B14" s="73"/>
       <c r="C14" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D14" s="63"/>
       <c r="E14" s="78"/>
@@ -4965,7 +4965,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F17" s="59" t="s">
         <v>8</v>
@@ -5007,7 +5007,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F18" s="59" t="s">
         <v>164</v>
@@ -5679,7 +5679,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5690,7 +5690,7 @@
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5772,7 +5772,7 @@
         <v>207</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
@@ -5846,11 +5846,11 @@
         <v>145</v>
       </c>
       <c r="D1" s="89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E1" s="90"/>
       <c r="F1" s="89" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G1" s="90"/>
     </row>
@@ -5905,11 +5905,11 @@
         <v>6</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G4" s="52"/>
     </row>

</xml_diff>

<commit_message>
support only file name in Java
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A4A07F-E41F-45D7-A6E9-EC2683FF2EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBBC6A7-9041-4BBD-BA5A-2C658BE4638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="230">
   <si>
     <t>Role</t>
   </si>
@@ -732,6 +732,12 @@
   </si>
   <si>
     <t>WrongWorksheet sheet does not exist.</t>
+  </si>
+  <si>
+    <t>Default Sheet</t>
+  </si>
+  <si>
+    <t>ExcelBDDSampleA.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1057,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1398,6 +1404,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4374,10 +4383,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93BB7E4-E9BF-490F-8356-65B5D0024489}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4395,9 +4404,10 @@
     <col min="11" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:15" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -4440,8 +4450,11 @@
       <c r="N1" s="6" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1">
+      <c r="O1" s="43" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -4460,32 +4473,35 @@
       <c r="F2" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="131" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="52" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -4502,32 +4518,33 @@
       <c r="F3" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="131" t="s">
         <v>184</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="131" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="131" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="30">
+      <c r="O3" s="52"/>
+    </row>
+    <row r="4" spans="1:15" ht="30">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -4544,26 +4561,29 @@
       <c r="F4" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7" t="s">
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7" t="s">
+      <c r="M4" s="131"/>
+      <c r="N4" s="131" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="131" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -4580,20 +4600,21 @@
       <c r="F5" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7" t="s">
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131" t="s">
         <v>226</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="131" t="s">
         <v>218</v>
       </c>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" ht="30">
+      <c r="N5" s="131"/>
+      <c r="O5" s="131"/>
+    </row>
+    <row r="6" spans="1:15" ht="30">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -4612,32 +4633,35 @@
       <c r="F6" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="131" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="131" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -4654,32 +4678,35 @@
       <c r="F7" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="131" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="131" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -4696,32 +4723,35 @@
       <c r="F8" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="131">
         <v>4.4000000000000004</v>
       </c>
-      <c r="N8" s="7" t="s">
+      <c r="N8" s="131" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="30">
+      <c r="O8" s="131">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -4738,32 +4768,35 @@
       <c r="F9" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="131" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="30">
+      <c r="O9" s="131" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -4780,32 +4813,35 @@
       <c r="F10" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="131" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" s="131" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -4822,16 +4858,17 @@
       <c r="F11" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" ht="30">
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="131"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="131"/>
+      <c r="M11" s="131"/>
+      <c r="N11" s="131"/>
+      <c r="O11" s="131"/>
+    </row>
+    <row r="12" spans="1:15" ht="30">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -4848,16 +4885,17 @@
       <c r="F12" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" ht="45">
+      <c r="G12" s="131"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="131"/>
+      <c r="J12" s="131"/>
+      <c r="K12" s="131"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="131"/>
+      <c r="N12" s="131"/>
+      <c r="O12" s="131"/>
+    </row>
+    <row r="13" spans="1:15" ht="45">
       <c r="A13" s="60">
         <v>12</v>
       </c>
@@ -4874,32 +4912,35 @@
       <c r="F13" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="131">
         <v>3</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="131">
         <v>3</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="131">
         <v>3</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="131">
         <v>3</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="131">
         <v>3</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="131">
         <v>3</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="131">
         <v>3</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="131">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13" s="131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="61"/>
       <c r="B14" s="73"/>
       <c r="C14" s="56" t="s">
@@ -4908,16 +4949,17 @@
       <c r="D14" s="63"/>
       <c r="E14" s="78"/>
       <c r="F14" s="75"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="G14" s="131"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="131"/>
+      <c r="L14" s="131"/>
+      <c r="M14" s="131"/>
+      <c r="N14" s="131"/>
+      <c r="O14" s="131"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="61"/>
       <c r="B15" s="73"/>
       <c r="C15" s="56" t="s">
@@ -4926,16 +4968,17 @@
       <c r="D15" s="63"/>
       <c r="E15" s="78"/>
       <c r="F15" s="75"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="G15" s="131"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="131"/>
+      <c r="M15" s="131"/>
+      <c r="N15" s="131"/>
+      <c r="O15" s="131"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="62"/>
       <c r="B16" s="73"/>
       <c r="C16" s="20" t="s">
@@ -4944,16 +4987,17 @@
       <c r="D16" s="63"/>
       <c r="E16" s="79"/>
       <c r="F16" s="76"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" ht="30">
+      <c r="G16" s="131"/>
+      <c r="H16" s="131"/>
+      <c r="I16" s="131"/>
+      <c r="J16" s="131"/>
+      <c r="K16" s="131"/>
+      <c r="L16" s="131"/>
+      <c r="M16" s="131"/>
+      <c r="N16" s="131"/>
+      <c r="O16" s="131"/>
+    </row>
+    <row r="17" spans="1:15" ht="30">
       <c r="A17" s="24">
         <v>13</v>
       </c>
@@ -4970,32 +5014,35 @@
       <c r="F17" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="131">
         <v>5</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="131">
         <v>5</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="131">
         <v>5</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="131">
         <v>5</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="131">
         <v>9</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="131">
         <v>13</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="131">
         <v>5</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="131">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17" s="131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -5012,28 +5059,31 @@
       <c r="F18" s="59" t="s">
         <v>164</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="131">
         <v>4</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="131">
         <v>4</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="131">
         <v>4</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="131">
         <v>4</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="131">
         <v>4</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="131">
         <v>5</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="131">
         <v>4</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="131">
+        <v>4</v>
+      </c>
+      <c r="O18" s="131">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
throw exception when missing parameter name grid
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBBC6A7-9041-4BBD-BA5A-2C658BE4638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE4B56D-AC7E-4B97-8E1A-173FB79B1FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="3" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="233">
   <si>
     <t>Role</t>
   </si>
@@ -738,6 +738,15 @@
   </si>
   <si>
     <t>ExcelBDDSampleA.xlsx</t>
+  </si>
+  <si>
+    <t>MissingGrid</t>
+  </si>
+  <si>
+    <t>Missing Parameter Name Grid, Wrong</t>
+  </si>
+  <si>
+    <t>Parameter Name grid is not found</t>
   </si>
 </sst>
 </file>
@@ -1192,6 +1201,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1404,9 +1416,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1943,7 +1952,7 @@
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="68" t="s">
         <v>210</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -1987,7 +1996,7 @@
       <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="22" t="s">
         <v>150</v>
       </c>
@@ -2029,7 +2038,7 @@
       <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="68"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="22" t="s">
         <v>25</v>
       </c>
@@ -2071,7 +2080,7 @@
       <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="68"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="22" t="s">
         <v>27</v>
       </c>
@@ -2111,7 +2120,7 @@
     </row>
     <row r="6" spans="1:14" ht="30">
       <c r="A6" s="21"/>
-      <c r="B6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="25" t="s">
         <v>89</v>
       </c>
@@ -2149,7 +2158,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="21"/>
-      <c r="B7" s="68"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="25" t="s">
         <v>215</v>
       </c>
@@ -2177,7 +2186,7 @@
       <c r="A8" s="21">
         <v>5</v>
       </c>
-      <c r="B8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="45" t="s">
         <v>178</v>
       </c>
@@ -2219,7 +2228,7 @@
       <c r="A9" s="21">
         <v>6</v>
       </c>
-      <c r="B9" s="69"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="47" t="s">
         <v>179</v>
       </c>
@@ -2261,7 +2270,7 @@
       <c r="A10" s="21">
         <v>7</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="71" t="s">
         <v>171</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -2305,7 +2314,7 @@
       <c r="A11" s="21">
         <v>8</v>
       </c>
-      <c r="B11" s="71"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="22" t="s">
         <v>31</v>
       </c>
@@ -2347,7 +2356,7 @@
       <c r="A12" s="21">
         <v>9</v>
       </c>
-      <c r="B12" s="71"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="22" t="s">
         <v>34</v>
       </c>
@@ -2389,7 +2398,7 @@
       <c r="A13" s="21">
         <v>10</v>
       </c>
-      <c r="B13" s="71"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="23" t="s">
         <v>68</v>
       </c>
@@ -2431,7 +2440,7 @@
       <c r="A14" s="21">
         <v>11</v>
       </c>
-      <c r="B14" s="71"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="23" t="s">
         <v>69</v>
       </c>
@@ -2473,7 +2482,7 @@
       <c r="A15" s="21">
         <v>12</v>
       </c>
-      <c r="B15" s="71"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="23" t="s">
         <v>66</v>
       </c>
@@ -2499,7 +2508,7 @@
       <c r="A16" s="21">
         <v>13</v>
       </c>
-      <c r="B16" s="71"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="22" t="s">
         <v>81</v>
       </c>
@@ -2522,20 +2531,20 @@
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" ht="45">
-      <c r="A17" s="60">
+      <c r="A17" s="61">
         <v>14</v>
       </c>
-      <c r="B17" s="71"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="64" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="65" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="7">
@@ -2564,16 +2573,16 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="61"/>
-      <c r="B18" s="71"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="64"/>
       <c r="E18" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F18" s="65"/>
+      <c r="F18" s="66"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -2584,16 +2593,16 @@
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="61"/>
-      <c r="B19" s="71"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="63"/>
+      <c r="D19" s="64"/>
       <c r="E19" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F19" s="65"/>
+      <c r="F19" s="66"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2604,16 +2613,16 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="62"/>
-      <c r="B20" s="71"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="63"/>
+      <c r="D20" s="64"/>
       <c r="E20" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F20" s="66"/>
+      <c r="F20" s="67"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2627,7 +2636,7 @@
       <c r="A21" s="24">
         <v>16</v>
       </c>
-      <c r="B21" s="71"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="25" t="s">
         <v>36</v>
       </c>
@@ -2669,7 +2678,7 @@
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="B22" s="72"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="41" t="s">
         <v>163</v>
       </c>
@@ -2739,42 +2748,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="118" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="118"/>
+      <c r="D1" s="119"/>
       <c r="E1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="122" t="s">
+      <c r="F1" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="127" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="127"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="125" t="s">
+      <c r="F2" s="126" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="127"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -2806,16 +2815,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="105" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="120" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2835,12 +2844,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="105"/>
+      <c r="A5" s="106"/>
       <c r="B5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="120"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="121"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2858,12 +2867,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="105"/>
+      <c r="A6" s="106"/>
       <c r="B6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="121"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="122"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2873,7 +2882,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="106"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="9" t="s">
         <v>60</v>
       </c>
@@ -2962,31 +2971,31 @@
       <c r="B1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="89" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="129" t="s">
+      <c r="J1" s="91"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="89" t="s">
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="128"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="129"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -3308,26 +3317,26 @@
       <c r="B1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="89" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="129" t="s">
+      <c r="J1" s="91"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3661,36 +3670,36 @@
       <c r="D1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="89" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="90"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="89" t="s">
+      <c r="I1" s="91"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="90"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="91" t="s">
+      <c r="L1" s="91"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="89" t="s">
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="R1" s="90"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="89" t="s">
+      <c r="R1" s="91"/>
+      <c r="S1" s="129"/>
+      <c r="T1" s="90" t="s">
         <v>162</v>
       </c>
-      <c r="U1" s="90"/>
-      <c r="V1" s="128"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="129"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -4076,24 +4085,24 @@
       <c r="B1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="89" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="89" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="I1" s="129" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="130"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="90"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -4385,7 +4394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93BB7E4-E9BF-490F-8356-65B5D0024489}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -4458,7 +4467,7 @@
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="68" t="s">
         <v>210</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -4473,28 +4482,28 @@
       <c r="F2" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="131" t="s">
+      <c r="G2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="131" t="s">
+      <c r="H2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="131" t="s">
+      <c r="J2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="K2" s="131" t="s">
+      <c r="K2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="L2" s="131" t="s">
+      <c r="L2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="131" t="s">
+      <c r="M2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="131" t="s">
+      <c r="N2" s="60" t="s">
         <v>159</v>
       </c>
       <c r="O2" s="52" t="s">
@@ -4505,7 +4514,7 @@
       <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="22" t="s">
         <v>150</v>
       </c>
@@ -4518,28 +4527,28 @@
       <c r="F3" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="131" t="s">
+      <c r="G3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="131" t="s">
+      <c r="I3" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="131" t="s">
+      <c r="J3" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="131" t="s">
+      <c r="K3" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="L3" s="131" t="s">
+      <c r="L3" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="131" t="s">
+      <c r="M3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="131" t="s">
+      <c r="N3" s="60" t="s">
         <v>188</v>
       </c>
       <c r="O3" s="52"/>
@@ -4548,7 +4557,7 @@
       <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="68"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="25" t="s">
         <v>89</v>
       </c>
@@ -4561,25 +4570,25 @@
       <c r="F4" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="131" t="s">
+      <c r="G4" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="131" t="s">
+      <c r="H4" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131" t="s">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="131" t="s">
+      <c r="L4" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="131"/>
-      <c r="N4" s="131" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="O4" s="131" t="s">
+      <c r="O4" s="60" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4587,7 +4596,7 @@
       <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="69"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="25" t="s">
         <v>215</v>
       </c>
@@ -4600,25 +4609,25 @@
       <c r="F5" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131" t="s">
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="M5" s="131" t="s">
+      <c r="M5" s="60" t="s">
         <v>218</v>
       </c>
-      <c r="N5" s="131"/>
-      <c r="O5" s="131"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="1:15" ht="30">
       <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="74" t="s">
         <v>171</v>
       </c>
       <c r="C6" s="54" t="s">
@@ -4633,31 +4642,31 @@
       <c r="F6" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="131" t="s">
+      <c r="G6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="131" t="s">
+      <c r="H6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="131" t="s">
+      <c r="I6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="131" t="s">
+      <c r="J6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="131" t="s">
+      <c r="K6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="131" t="s">
+      <c r="L6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="131" t="s">
+      <c r="M6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="131" t="s">
+      <c r="N6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="131" t="s">
+      <c r="O6" s="60" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4665,7 +4674,7 @@
       <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="73"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="54" t="s">
         <v>31</v>
       </c>
@@ -4678,31 +4687,31 @@
       <c r="F7" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="131" t="s">
+      <c r="H7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="131" t="s">
+      <c r="I7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="131" t="s">
+      <c r="J7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="131" t="s">
+      <c r="K7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="131" t="s">
+      <c r="L7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="131" t="s">
+      <c r="M7" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="131" t="s">
+      <c r="N7" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="O7" s="131" t="s">
+      <c r="O7" s="60" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4710,7 +4719,7 @@
       <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="54" t="s">
         <v>34</v>
       </c>
@@ -4723,31 +4732,31 @@
       <c r="F8" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="131">
+      <c r="G8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H8" s="131">
+      <c r="H8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I8" s="131">
+      <c r="I8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J8" s="131">
+      <c r="J8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K8" s="131">
+      <c r="K8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L8" s="131">
+      <c r="L8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M8" s="131">
+      <c r="M8" s="60">
         <v>4.4000000000000004</v>
       </c>
-      <c r="N8" s="131" t="s">
+      <c r="N8" s="60" t="s">
         <v>224</v>
       </c>
-      <c r="O8" s="131">
+      <c r="O8" s="60">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -4755,7 +4764,7 @@
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="73"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="55" t="s">
         <v>68</v>
       </c>
@@ -4768,31 +4777,31 @@
       <c r="F9" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="131" t="s">
+      <c r="G9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="131" t="s">
+      <c r="H9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="131" t="s">
+      <c r="I9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="131" t="s">
+      <c r="J9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="131" t="s">
+      <c r="K9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="131" t="s">
+      <c r="L9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="131" t="s">
+      <c r="M9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="131" t="s">
+      <c r="N9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="131" t="s">
+      <c r="O9" s="60" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4800,7 +4809,7 @@
       <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="73"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="55" t="s">
         <v>69</v>
       </c>
@@ -4813,31 +4822,31 @@
       <c r="F10" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="131" t="s">
+      <c r="G10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="131" t="s">
+      <c r="H10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="131" t="s">
+      <c r="I10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="131" t="s">
+      <c r="J10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="131" t="s">
+      <c r="K10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="131" t="s">
+      <c r="L10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="131" t="s">
+      <c r="M10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="131" t="s">
+      <c r="N10" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="131" t="s">
+      <c r="O10" s="60" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4845,7 +4854,7 @@
       <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="73"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="55" t="s">
         <v>66</v>
       </c>
@@ -4858,21 +4867,21 @@
       <c r="F11" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="131"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="131"/>
-      <c r="M11" s="131"/>
-      <c r="N11" s="131"/>
-      <c r="O11" s="131"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="30">
       <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="73"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="54" t="s">
         <v>81</v>
       </c>
@@ -4885,123 +4894,123 @@
       <c r="F12" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="131"/>
-      <c r="H12" s="131"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="131"/>
-      <c r="N12" s="131"/>
-      <c r="O12" s="131"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
     </row>
     <row r="13" spans="1:15" ht="45">
-      <c r="A13" s="60">
+      <c r="A13" s="61">
         <v>12</v>
       </c>
-      <c r="B13" s="73"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="131">
+      <c r="G13" s="60">
         <v>3</v>
       </c>
-      <c r="H13" s="131">
+      <c r="H13" s="60">
         <v>3</v>
       </c>
-      <c r="I13" s="131">
+      <c r="I13" s="60">
         <v>3</v>
       </c>
-      <c r="J13" s="131">
+      <c r="J13" s="60">
         <v>3</v>
       </c>
-      <c r="K13" s="131">
+      <c r="K13" s="60">
         <v>3</v>
       </c>
-      <c r="L13" s="131">
+      <c r="L13" s="60">
         <v>3</v>
       </c>
-      <c r="M13" s="131">
+      <c r="M13" s="60">
         <v>3</v>
       </c>
-      <c r="N13" s="131">
+      <c r="N13" s="60">
         <v>3</v>
       </c>
-      <c r="O13" s="131">
+      <c r="O13" s="60">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="61"/>
-      <c r="B14" s="73"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="131"/>
-      <c r="H14" s="131"/>
-      <c r="I14" s="131"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="131"/>
-      <c r="M14" s="131"/>
-      <c r="N14" s="131"/>
-      <c r="O14" s="131"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="61"/>
-      <c r="B15" s="73"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="131"/>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="131"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="131"/>
-      <c r="O15" s="131"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="62"/>
-      <c r="B16" s="73"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="131"/>
-      <c r="O16" s="131"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
     </row>
     <row r="17" spans="1:15" ht="30">
       <c r="A17" s="24">
         <v>13</v>
       </c>
-      <c r="B17" s="73"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="57" t="s">
         <v>36</v>
       </c>
@@ -5014,31 +5023,31 @@
       <c r="F17" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="131">
+      <c r="G17" s="60">
         <v>5</v>
       </c>
-      <c r="H17" s="131">
+      <c r="H17" s="60">
         <v>5</v>
       </c>
-      <c r="I17" s="131">
+      <c r="I17" s="60">
         <v>5</v>
       </c>
-      <c r="J17" s="131">
+      <c r="J17" s="60">
         <v>5</v>
       </c>
-      <c r="K17" s="131">
+      <c r="K17" s="60">
         <v>9</v>
       </c>
-      <c r="L17" s="131">
+      <c r="L17" s="60">
         <v>13</v>
       </c>
-      <c r="M17" s="131">
+      <c r="M17" s="60">
         <v>5</v>
       </c>
-      <c r="N17" s="131">
+      <c r="N17" s="60">
         <v>13</v>
       </c>
-      <c r="O17" s="131">
+      <c r="O17" s="60">
         <v>5</v>
       </c>
     </row>
@@ -5046,7 +5055,7 @@
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="73"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="58" t="s">
         <v>163</v>
       </c>
@@ -5059,31 +5068,31 @@
       <c r="F18" s="59" t="s">
         <v>164</v>
       </c>
-      <c r="G18" s="131">
+      <c r="G18" s="60">
         <v>4</v>
       </c>
-      <c r="H18" s="131">
+      <c r="H18" s="60">
         <v>4</v>
       </c>
-      <c r="I18" s="131">
+      <c r="I18" s="60">
         <v>4</v>
       </c>
-      <c r="J18" s="131">
+      <c r="J18" s="60">
         <v>4</v>
       </c>
-      <c r="K18" s="131">
+      <c r="K18" s="60">
         <v>4</v>
       </c>
-      <c r="L18" s="131">
+      <c r="L18" s="60">
         <v>5</v>
       </c>
-      <c r="M18" s="131">
+      <c r="M18" s="60">
         <v>4</v>
       </c>
-      <c r="N18" s="131">
+      <c r="N18" s="60">
         <v>4</v>
       </c>
-      <c r="O18" s="131">
+      <c r="O18" s="60">
         <v>4</v>
       </c>
     </row>
@@ -5126,41 +5135,41 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="86" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="88" t="s">
         <v>158</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="80" t="s">
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
       <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
@@ -5184,7 +5193,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="83" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -5222,7 +5231,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="82"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="22" t="s">
         <v>150</v>
       </c>
@@ -5258,7 +5267,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="82"/>
+      <c r="A7" s="83"/>
       <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
@@ -5294,7 +5303,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="82"/>
+      <c r="A8" s="83"/>
       <c r="B8" s="22" t="s">
         <v>27</v>
       </c>
@@ -5330,7 +5339,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="82"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="22" t="s">
         <v>178</v>
       </c>
@@ -5366,7 +5375,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="82"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="42" t="s">
         <v>179</v>
       </c>
@@ -5402,7 +5411,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="85" t="s">
         <v>171</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -5434,7 +5443,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="84"/>
+      <c r="A12" s="85"/>
       <c r="B12" s="22" t="s">
         <v>151</v>
       </c>
@@ -5470,7 +5479,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="84"/>
+      <c r="A13" s="85"/>
       <c r="B13" s="22" t="s">
         <v>152</v>
       </c>
@@ -5502,7 +5511,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="84"/>
+      <c r="A14" s="85"/>
       <c r="B14" s="22" t="s">
         <v>153</v>
       </c>
@@ -5534,7 +5543,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="84"/>
+      <c r="A15" s="85"/>
       <c r="B15" s="23" t="s">
         <v>154</v>
       </c>
@@ -5570,8 +5579,8 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="84"/>
-      <c r="B16" s="83" t="s">
+      <c r="A16" s="85"/>
+      <c r="B16" s="84" t="s">
         <v>175</v>
       </c>
       <c r="C16" s="24" t="s">
@@ -5608,8 +5617,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="84"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="84"/>
       <c r="C17" s="24" t="s">
         <v>5</v>
       </c>
@@ -5644,8 +5653,8 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="84"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="84"/>
       <c r="C18" s="24" t="s">
         <v>5</v>
       </c>
@@ -5670,8 +5679,8 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="84"/>
-      <c r="B19" s="83"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="24" t="s">
         <v>5</v>
       </c>
@@ -5726,10 +5735,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4E5E2-8FAC-4516-9FEA-053724A7E1DD}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5741,24 +5750,30 @@
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="92" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="89" t="s">
+      <c r="E1" s="92"/>
+      <c r="F1" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="90"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="91"/>
+      <c r="H1" s="90" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="91"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -5780,9 +5795,15 @@
       <c r="G2" s="35" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="73" t="s">
+      <c r="H2" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="74" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -5803,9 +5824,15 @@
       <c r="G3" s="52" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="73"/>
+      <c r="H3" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="74"/>
       <c r="B4" s="22" t="s">
         <v>150</v>
       </c>
@@ -5824,9 +5851,15 @@
       <c r="G4" s="52" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="73"/>
+      <c r="H4" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="I4" s="52" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="74"/>
       <c r="B5" s="22" t="s">
         <v>25</v>
       </c>
@@ -5841,9 +5874,15 @@
         <v>1</v>
       </c>
       <c r="G5" s="52"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="73"/>
+      <c r="H5" s="50">
+        <v>7</v>
+      </c>
+      <c r="I5" s="52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="74"/>
       <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
@@ -5858,12 +5897,19 @@
         <v>208</v>
       </c>
       <c r="G6" s="52"/>
+      <c r="H6" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="52">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5875,7 +5921,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H2" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5895,14 +5941,14 @@
       <c r="C1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="90" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="90"/>
-      <c r="F1" s="89" t="s">
+      <c r="E1" s="91"/>
+      <c r="F1" s="90" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="90"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
@@ -5928,7 +5974,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="74" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -5947,7 +5993,7 @@
       <c r="G3" s="52"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="73"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="22" t="s">
         <v>150</v>
       </c>
@@ -5964,7 +6010,7 @@
       <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="73"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="22" t="s">
         <v>25</v>
       </c>
@@ -5985,7 +6031,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="73"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
@@ -6037,41 +6083,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="107" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="108" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="108" t="s">
+      <c r="B2" s="114"/>
+      <c r="C2" s="109" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="110"/>
+      <c r="C3" s="111"/>
       <c r="D3" s="13" t="s">
         <v>110</v>
       </c>
@@ -6098,14 +6144,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="29" t="s">
         <v>102</v>
       </c>
@@ -6129,11 +6175,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="105"/>
-      <c r="B5" s="111" t="s">
+      <c r="A5" s="106"/>
+      <c r="B5" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="111"/>
+      <c r="C5" s="112"/>
       <c r="D5" s="33" t="s">
         <v>112</v>
       </c>
@@ -6160,12 +6206,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="105"/>
-      <c r="B6" s="101" t="s">
+      <c r="A6" s="106"/>
+      <c r="B6" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="104"/>
       <c r="E6" s="29" t="s">
         <v>108</v>
       </c>
@@ -6189,11 +6235,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="105"/>
-      <c r="B7" s="92" t="s">
+      <c r="A7" s="106"/>
+      <c r="B7" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="33" t="s">
         <v>113</v>
       </c>
@@ -6220,9 +6266,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="105"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="95"/>
+      <c r="A8" s="106"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="34" t="s">
         <v>119</v>
       </c>
@@ -6249,9 +6295,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="105"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="95"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="33" t="s">
         <v>120</v>
       </c>
@@ -6278,9 +6324,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="106"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="97"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="98"/>
       <c r="D10" s="33" t="s">
         <v>121</v>
       </c>
@@ -6438,7 +6484,7 @@
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="114" t="s">
+      <c r="A7" s="115" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -6451,7 +6497,7 @@
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="115"/>
+      <c r="A8" s="116"/>
       <c r="B8" s="4" t="s">
         <v>82</v>
       </c>
@@ -6462,7 +6508,7 @@
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="117" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -6485,7 +6531,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="117"/>
+      <c r="A10" s="118"/>
       <c r="B10" s="15" t="s">
         <v>82</v>
       </c>
@@ -6758,15 +6804,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -6802,7 +6848,7 @@
       <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="120" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -6828,7 +6874,7 @@
       <c r="B4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="120"/>
+      <c r="C4" s="121"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -6852,7 +6898,7 @@
       <c r="B5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="121"/>
+      <c r="C5" s="122"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
handle missing parameter name grid in PS
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE4B56D-AC7E-4B97-8E1A-173FB79B1FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CCEF31-0327-477C-8BEC-C5DBF9A35183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="3" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="7" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -4395,7 +4395,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5737,7 +5737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4E5E2-8FAC-4516-9FEA-053724A7E1DD}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -6576,8 +6576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A494DA1E-3A4D-414E-886D-A717DFF21DE7}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
upgrade PS to V0.4.1
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E76A7C-FCCF-4CBE-AA8D-D0A51A88538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1A9268-C49C-4ABD-94A3-E4685F18A988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="3" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="238">
   <si>
     <t>Role</t>
   </si>
@@ -747,13 +747,28 @@
   </si>
   <si>
     <t>Parameter Name grid is not found</t>
+  </si>
+  <si>
+    <t>select sheet,if not set, select 1st sheet</t>
+  </si>
+  <si>
+    <t>select test data set according to matcher,if not, match all</t>
+  </si>
+  <si>
+    <t>select test data set to avoid unmatcher,if not, exclude nothing</t>
+  </si>
+  <si>
+    <t>SBT3</t>
+  </si>
+  <si>
+    <t>SBTSheet3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,8 +833,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -888,6 +918,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,7 +1102,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1089,7 +1125,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1183,27 +1218,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1246,24 +1260,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1416,6 +1412,97 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1882,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1949,19 +2036,19 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="60" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -1993,17 +2080,17 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="21">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -2035,17 +2122,17 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="61"/>
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -2077,17 +2164,17 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="30">
-      <c r="A5" s="21">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -2119,18 +2206,18 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="30">
-      <c r="A6" s="21"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="25" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="52" t="s">
         <v>95</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -2157,18 +2244,18 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="21"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="52" t="s">
         <v>217</v>
       </c>
       <c r="G7" s="7"/>
@@ -2183,17 +2270,17 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>5</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="45" t="s">
         <v>174</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -2225,20 +2312,20 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="21">
+      <c r="A9" s="20">
         <v>6</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="47" t="s">
+      <c r="B9" s="62"/>
+      <c r="C9" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="42" t="s">
         <v>181</v>
       </c>
       <c r="G9" s="7" t="s">
@@ -2267,19 +2354,19 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="30">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>7</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -2311,17 +2398,17 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>8</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="64"/>
+      <c r="C11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -2353,17 +2440,17 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>9</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="64"/>
+      <c r="C12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -2395,17 +2482,17 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="30">
-      <c r="A13" s="21">
+      <c r="A13" s="20">
         <v>10</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="64"/>
+      <c r="C13" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -2437,17 +2524,17 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="30">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>11</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="23" t="s">
+      <c r="B14" s="64"/>
+      <c r="C14" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -2479,17 +2566,17 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="21">
+      <c r="A15" s="20">
         <v>12</v>
       </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -2505,17 +2592,17 @@
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="30">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>13</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -2531,20 +2618,20 @@
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" ht="45">
-      <c r="A17" s="61">
+      <c r="A17" s="53">
         <v>14</v>
       </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F17" s="65" t="s">
+      <c r="F17" s="57" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="7">
@@ -2573,16 +2660,16 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="62"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="19" t="s">
+      <c r="A18" s="54"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="24" t="s">
+      <c r="D18" s="56"/>
+      <c r="E18" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F18" s="66"/>
+      <c r="F18" s="58"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -2593,16 +2680,16 @@
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="62"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="19" t="s">
+      <c r="A19" s="54"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="24" t="s">
+      <c r="D19" s="56"/>
+      <c r="E19" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F19" s="66"/>
+      <c r="F19" s="58"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2613,16 +2700,16 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="63"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="20" t="s">
+      <c r="A20" s="55"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="24" t="s">
+      <c r="D20" s="56"/>
+      <c r="E20" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F20" s="67"/>
+      <c r="F20" s="59"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2633,44 +2720,44 @@
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:14" ht="30">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <v>16</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="25" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="47">
         <v>5</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="47">
         <v>5</v>
       </c>
-      <c r="I21" s="48">
+      <c r="I21" s="47">
         <v>5</v>
       </c>
-      <c r="J21" s="48">
+      <c r="J21" s="47">
         <v>5</v>
       </c>
-      <c r="K21" s="48">
+      <c r="K21" s="47">
         <v>9</v>
       </c>
-      <c r="L21" s="48">
+      <c r="L21" s="47">
         <v>13</v>
       </c>
-      <c r="M21" s="48">
+      <c r="M21" s="47">
         <v>5</v>
       </c>
-      <c r="N21" s="48">
+      <c r="N21" s="47">
         <v>13</v>
       </c>
     </row>
@@ -2678,14 +2765,14 @@
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="B22" s="73"/>
-      <c r="C22" s="41" t="s">
+      <c r="B22" s="65"/>
+      <c r="C22" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="23" t="s">
         <v>173</v>
       </c>
       <c r="F22" s="6" t="s">
@@ -2735,7 +2822,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2748,57 +2835,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="119" t="s">
+      <c r="B1" s="111"/>
+      <c r="C1" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="119"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="105"/>
+      <c r="E1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="128" t="s">
+      <c r="B2" s="111"/>
+      <c r="C2" s="114" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="128"/>
+      <c r="D2" s="114"/>
       <c r="E2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="126" t="s">
+      <c r="F2" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="127"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>78</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -2815,16 +2902,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="91" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="106" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2844,12 +2931,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="106"/>
+      <c r="A5" s="92"/>
       <c r="B5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="121"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2867,12 +2954,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="106"/>
+      <c r="A6" s="92"/>
       <c r="B6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="107"/>
-      <c r="D6" s="122"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2882,7 +2969,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="107"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="9" t="s">
         <v>60</v>
       </c>
@@ -2895,13 +2982,13 @@
       <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>99</v>
       </c>
       <c r="G7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="27" t="b">
+      <c r="H7" s="26" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="7">
@@ -2951,7 +3038,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2968,34 +3055,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="90" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="90" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="91"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="130" t="s">
+      <c r="J1" s="77"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
-      <c r="O1" s="90" t="s">
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="129"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="115"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -3004,54 +3091,54 @@
       <c r="B2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="P2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="34" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3109,7 +3196,7 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3167,7 +3254,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3200,13 +3287,13 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D6" s="8" t="str">
@@ -3226,7 +3313,7 @@
       <c r="H6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="I6" s="27" t="b">
+      <c r="I6" s="26" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="8" t="b">
@@ -3314,29 +3401,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="90" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="90" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="91"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="130" t="s">
+      <c r="J1" s="77"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3345,61 +3432,61 @@
       <c r="B2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="34" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3447,7 +3534,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="21"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
         <v>82</v>
       </c>
@@ -3457,12 +3544,12 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">
@@ -3472,7 +3559,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -3482,12 +3569,12 @@
       <c r="C7" s="4"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -3535,7 +3622,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3563,13 +3650,13 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="37" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D10" s="8" t="str">
@@ -3589,7 +3676,7 @@
       <c r="H10" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="I10" s="27" t="b">
+      <c r="I10" s="26" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="8" t="b">
@@ -3667,39 +3754,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="90" t="s">
+      <c r="F1" s="77"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="91"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="90" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="92" t="s">
+      <c r="L1" s="77"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="90" t="s">
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="R1" s="91"/>
-      <c r="S1" s="129"/>
-      <c r="T1" s="90" t="s">
+      <c r="R1" s="77"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="U1" s="91"/>
-      <c r="V1" s="129"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="115"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -3714,58 +3801,58 @@
       <c r="D2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="P2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="S2" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="U2" s="35" t="s">
+      <c r="U2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="V2" s="35" t="s">
+      <c r="V2" s="34" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3773,10 +3860,10 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
@@ -3845,10 +3932,10 @@
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -3917,10 +4004,10 @@
       <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -3959,14 +4046,14 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>99</v>
       </c>
       <c r="F6" s="8" t="str">
@@ -3986,7 +4073,7 @@
       <c r="J6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="K6" s="27" t="b">
+      <c r="K6" s="26" t="b">
         <v>1</v>
       </c>
       <c r="L6" s="8" t="b">
@@ -4016,7 +4103,7 @@
       <c r="S6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="T6" s="28" t="s">
+      <c r="T6" s="27" t="s">
         <v>99</v>
       </c>
       <c r="U6" s="8" t="str">
@@ -4070,7 +4157,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4082,27 +4169,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="90" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="90" t="s">
+      <c r="F1" s="77"/>
+      <c r="G1" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="91"/>
-      <c r="I1" s="130" t="s">
+      <c r="H1" s="77"/>
+      <c r="I1" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="131"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -4111,35 +4198,35 @@
       <c r="B2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4177,7 +4264,7 @@
       <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -4215,7 +4302,7 @@
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -4233,13 +4320,13 @@
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D6" s="8" t="str">
@@ -4253,7 +4340,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="27" t="b">
+      <c r="G6" s="26" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="b">
@@ -4328,7 +4415,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4371,7 +4458,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>199</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4392,10 +4479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93BB7E4-E9BF-490F-8356-65B5D0024489}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4404,7 +4491,7 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
@@ -4414,686 +4501,729 @@
     <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" ht="47.25">
+      <c r="A1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="119" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="118" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="119" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="119" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="119" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="119" t="s">
         <v>219</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="119" t="s">
         <v>225</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="121" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1">
-      <c r="A2" s="21">
+      <c r="P1" s="121" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1">
+      <c r="A2" s="122">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="123" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="124" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="125" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="126" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="60" t="s">
+      <c r="N2" s="127" t="s">
         <v>159</v>
       </c>
-      <c r="O2" s="52" t="s">
+      <c r="O2" s="128" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="21">
+      <c r="P2" s="127" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="31.5">
+      <c r="A3" s="122">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="B3" s="129"/>
+      <c r="C3" s="124" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="125" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="127" t="s">
         <v>184</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="L3" s="127" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="127" t="s">
         <v>188</v>
       </c>
-      <c r="O3" s="52"/>
-    </row>
-    <row r="4" spans="1:15" ht="30">
-      <c r="A4" s="21">
+      <c r="O3" s="128"/>
+      <c r="P3" s="128" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="31.5">
+      <c r="A4" s="122">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="130" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="125" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60" t="s">
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="60" t="s">
+      <c r="L4" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60" t="s">
+      <c r="M4" s="127"/>
+      <c r="N4" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="O4" s="60" t="s">
+      <c r="O4" s="127" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="21">
+      <c r="P4" s="127" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="31.5">
+      <c r="A5" s="122">
         <v>4</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="24" t="s">
+      <c r="B5" s="132"/>
+      <c r="C5" s="130" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="125" t="s">
         <v>148</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="131" t="s">
         <v>217</v>
       </c>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60" t="s">
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127" t="s">
         <v>226</v>
       </c>
-      <c r="M5" s="60" t="s">
+      <c r="M5" s="127" t="s">
         <v>218</v>
       </c>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-    </row>
-    <row r="6" spans="1:15" ht="30">
-      <c r="A6" s="21">
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+    </row>
+    <row r="6" spans="1:16" ht="31.5">
+      <c r="A6" s="122">
         <v>5</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="133" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="60" t="s">
+      <c r="K6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="60" t="s">
+      <c r="M6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="60" t="s">
+      <c r="N6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="60" t="s">
+      <c r="O6" s="127" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="21">
+      <c r="P6" s="127" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75">
+      <c r="A7" s="122">
         <v>6</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="54" t="s">
+      <c r="B7" s="133"/>
+      <c r="C7" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="60" t="s">
+      <c r="H7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="60" t="s">
+      <c r="I7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="60" t="s">
+      <c r="K7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="60" t="s">
+      <c r="L7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="60" t="s">
+      <c r="M7" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="60" t="s">
+      <c r="N7" s="127" t="s">
         <v>223</v>
       </c>
-      <c r="O7" s="60" t="s">
+      <c r="O7" s="127" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="21">
+      <c r="P7" s="127" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75">
+      <c r="A8" s="122">
         <v>7</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="54" t="s">
+      <c r="B8" s="133"/>
+      <c r="C8" s="134" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="60">
+      <c r="G8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I8" s="60">
+      <c r="I8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J8" s="60">
+      <c r="J8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="K8" s="60">
+      <c r="K8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L8" s="60">
+      <c r="L8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M8" s="60">
+      <c r="M8" s="127">
         <v>4.4000000000000004</v>
       </c>
-      <c r="N8" s="60" t="s">
+      <c r="N8" s="127" t="s">
         <v>224</v>
       </c>
-      <c r="O8" s="60">
+      <c r="O8" s="127">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="30">
-      <c r="A9" s="21">
+      <c r="P8" s="127">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="31.5">
+      <c r="A9" s="122">
         <v>8</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="55" t="s">
+      <c r="B9" s="133"/>
+      <c r="C9" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="60" t="s">
+      <c r="H9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="60" t="s">
+      <c r="K9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="60" t="s">
+      <c r="L9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="60" t="s">
+      <c r="M9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="60" t="s">
+      <c r="N9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="60" t="s">
+      <c r="O9" s="127" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="30">
-      <c r="A10" s="21">
+      <c r="P9" s="127" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="31.5">
+      <c r="A10" s="122">
         <v>9</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="55" t="s">
+      <c r="B10" s="133"/>
+      <c r="C10" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="60" t="s">
+      <c r="L10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="60" t="s">
+      <c r="O10" s="127" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="21">
+      <c r="P10" s="127" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="31.5">
+      <c r="A11" s="122">
         <v>10</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="55" t="s">
+      <c r="B11" s="133"/>
+      <c r="C11" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-    </row>
-    <row r="12" spans="1:15" ht="30">
-      <c r="A12" s="21">
+      <c r="G11" s="127"/>
+      <c r="H11" s="127"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="127"/>
+      <c r="K11" s="127"/>
+      <c r="L11" s="127"/>
+      <c r="M11" s="127"/>
+      <c r="N11" s="127"/>
+      <c r="O11" s="127"/>
+      <c r="P11" s="127"/>
+    </row>
+    <row r="12" spans="1:16" ht="31.5">
+      <c r="A12" s="122">
         <v>11</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="54" t="s">
+      <c r="B12" s="133"/>
+      <c r="C12" s="134" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F12" s="59" t="s">
+      <c r="F12" s="126" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-    </row>
-    <row r="13" spans="1:15" ht="45">
-      <c r="A13" s="61">
+      <c r="G12" s="127"/>
+      <c r="H12" s="127"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="127"/>
+      <c r="N12" s="127"/>
+      <c r="O12" s="127"/>
+      <c r="P12" s="127"/>
+    </row>
+    <row r="13" spans="1:16" ht="47.25">
+      <c r="A13" s="135">
         <v>12</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="54" t="s">
+      <c r="B13" s="133"/>
+      <c r="C13" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="137" t="s">
         <v>214</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="138" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="60">
+      <c r="G13" s="127">
         <v>3</v>
       </c>
-      <c r="H13" s="60">
+      <c r="H13" s="127">
         <v>3</v>
       </c>
-      <c r="I13" s="60">
+      <c r="I13" s="127">
         <v>3</v>
       </c>
-      <c r="J13" s="60">
+      <c r="J13" s="127">
         <v>3</v>
       </c>
-      <c r="K13" s="60">
+      <c r="K13" s="127">
         <v>3</v>
       </c>
-      <c r="L13" s="60">
+      <c r="L13" s="127">
         <v>3</v>
       </c>
-      <c r="M13" s="60">
+      <c r="M13" s="127">
         <v>3</v>
       </c>
-      <c r="N13" s="60">
+      <c r="N13" s="127">
         <v>3</v>
       </c>
-      <c r="O13" s="60">
+      <c r="O13" s="127">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="62"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="56" t="s">
+      <c r="P13" s="127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="31.5">
+      <c r="A14" s="139"/>
+      <c r="B14" s="133"/>
+      <c r="C14" s="140" t="s">
         <v>216</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="62"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="56" t="s">
+      <c r="D14" s="136"/>
+      <c r="E14" s="141"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="127"/>
+      <c r="O14" s="127"/>
+      <c r="P14" s="127"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75">
+      <c r="A15" s="139"/>
+      <c r="B15" s="133"/>
+      <c r="C15" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="63"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="20" t="s">
+      <c r="D15" s="136"/>
+      <c r="E15" s="141"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="127"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
+      <c r="K15" s="127"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="127"/>
+      <c r="O15" s="127"/>
+      <c r="P15" s="127"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75">
+      <c r="A16" s="143"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-    </row>
-    <row r="17" spans="1:15" ht="30">
-      <c r="A17" s="24">
+      <c r="D16" s="136"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="127"/>
+      <c r="O16" s="127"/>
+      <c r="P16" s="127"/>
+    </row>
+    <row r="17" spans="1:16" ht="31.5">
+      <c r="A17" s="125">
         <v>13</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="57" t="s">
+      <c r="B17" s="133"/>
+      <c r="C17" s="147" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F17" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="60">
+      <c r="G17" s="127">
         <v>5</v>
       </c>
-      <c r="H17" s="60">
+      <c r="H17" s="127">
         <v>5</v>
       </c>
-      <c r="I17" s="60">
+      <c r="I17" s="127">
         <v>5</v>
       </c>
-      <c r="J17" s="60">
+      <c r="J17" s="127">
         <v>5</v>
       </c>
-      <c r="K17" s="60">
+      <c r="K17" s="127">
         <v>9</v>
       </c>
-      <c r="L17" s="60">
+      <c r="L17" s="127">
         <v>13</v>
       </c>
-      <c r="M17" s="60">
+      <c r="M17" s="127">
         <v>5</v>
       </c>
-      <c r="N17" s="60">
+      <c r="N17" s="127">
         <v>13</v>
       </c>
-      <c r="O17" s="60">
+      <c r="O17" s="127">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="2">
+      <c r="P17" s="127">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="31.5">
+      <c r="A18" s="148">
         <v>14</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="58" t="s">
+      <c r="B18" s="133"/>
+      <c r="C18" s="149" t="s">
         <v>163</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="125" t="s">
         <v>214</v>
       </c>
-      <c r="F18" s="59" t="s">
+      <c r="F18" s="126" t="s">
         <v>164</v>
       </c>
-      <c r="G18" s="60">
+      <c r="G18" s="127">
         <v>4</v>
       </c>
-      <c r="H18" s="60">
+      <c r="H18" s="127">
         <v>4</v>
       </c>
-      <c r="I18" s="60">
+      <c r="I18" s="127">
         <v>4</v>
       </c>
-      <c r="J18" s="60">
+      <c r="J18" s="127">
         <v>4</v>
       </c>
-      <c r="K18" s="60">
+      <c r="K18" s="127">
         <v>4</v>
       </c>
-      <c r="L18" s="60">
+      <c r="L18" s="127">
         <v>5</v>
       </c>
-      <c r="M18" s="60">
+      <c r="M18" s="127">
         <v>4</v>
       </c>
-      <c r="N18" s="60">
+      <c r="N18" s="127">
         <v>4</v>
       </c>
-      <c r="O18" s="60">
+      <c r="O18" s="127">
         <v>4</v>
+      </c>
+      <c r="P18" s="127">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -5135,83 +5265,83 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="74" t="s">
         <v>158</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="81" t="s">
+      <c r="G3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="81" t="s">
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="67" t="s">
         <v>185</v>
       </c>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="87"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
+      <c r="A4" s="73"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
       <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="34" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="38" t="s">
         <v>159</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5220,7 +5350,7 @@
       <c r="I5" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="38" t="s">
         <v>159</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -5231,23 +5361,23 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="83"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="69"/>
+      <c r="B6" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>2</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="38" t="s">
         <v>140</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5256,7 +5386,7 @@
       <c r="I6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="38" t="s">
         <v>184</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -5267,23 +5397,23 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="83"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="69"/>
+      <c r="B7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>3</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="38">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5292,7 +5422,7 @@
       <c r="I7" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="38">
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -5303,23 +5433,23 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="83"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="69"/>
+      <c r="B8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>4</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="38" t="s">
         <v>37</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5328,7 +5458,7 @@
       <c r="I8" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="38" t="s">
         <v>37</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -5339,23 +5469,23 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="83"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="69"/>
+      <c r="B9" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <v>5</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>182</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -5364,7 +5494,7 @@
       <c r="I9" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="38" t="s">
         <v>182</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -5375,35 +5505,35 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="83"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="69"/>
+      <c r="B10" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>6</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="43" t="s">
         <v>160</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="K10" s="44" t="s">
+      <c r="K10" s="43" t="s">
         <v>160</v>
       </c>
       <c r="L10" s="8" t="s">
@@ -5411,31 +5541,31 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="71" t="s">
         <v>171</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="20">
         <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="38" t="s">
         <v>3</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="38" t="s">
         <v>3</v>
       </c>
       <c r="L11" s="8" t="s">
@@ -5443,23 +5573,23 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="85"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>8</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="38" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -5468,7 +5598,7 @@
       <c r="I12" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="38" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -5479,31 +5609,31 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="85"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="20">
         <v>9</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="38" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>144</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="38" t="s">
         <v>15</v>
       </c>
       <c r="L13" s="8" t="s">
@@ -5511,31 +5641,31 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="85"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>10</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>155</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="38" t="s">
         <v>18</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>144</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="38" t="s">
         <v>18</v>
       </c>
       <c r="L14" s="8" t="s">
@@ -5543,23 +5673,23 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="85"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="71"/>
+      <c r="B15" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>11</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="38" t="s">
         <v>156</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -5568,7 +5698,7 @@
       <c r="I15" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="38" t="s">
         <v>156</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -5579,17 +5709,17 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="85"/>
-      <c r="B16" s="84" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>12</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -5617,15 +5747,15 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="85"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="24" t="s">
+      <c r="A17" s="71"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>13</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -5653,15 +5783,15 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="85"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="24" t="s">
+      <c r="A18" s="71"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <v>14</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -5679,15 +5809,15 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="85"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="24" t="s">
+      <c r="A19" s="71"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="20">
         <v>15</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -5737,7 +5867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4E5E2-8FAC-4516-9FEA-053724A7E1DD}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -5757,21 +5887,21 @@
     <row r="1" spans="1:9">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="92"/>
-      <c r="F1" s="90" t="s">
+      <c r="E1" s="78"/>
+      <c r="F1" s="76" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="90" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="I1" s="91"/>
+      <c r="I1" s="77"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
@@ -5783,57 +5913,57 @@
       <c r="C2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="49" t="s">
         <v>229</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="51" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="74"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="66"/>
+      <c r="B4" s="21" t="s">
         <v>150</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -5842,65 +5972,65 @@
       <c r="D4" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="51" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="74"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="49">
         <v>1</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="50">
+      <c r="E5" s="51"/>
+      <c r="F5" s="49">
         <v>1</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="50">
+      <c r="G5" s="51"/>
+      <c r="H5" s="49">
         <v>7</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="51">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="74"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="66"/>
+      <c r="B6" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="50" t="s">
+      <c r="E6" s="51"/>
+      <c r="F6" s="49" t="s">
         <v>208</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="50" t="s">
+      <c r="G6" s="51"/>
+      <c r="H6" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="51">
         <v>4</v>
       </c>
     </row>
@@ -5938,17 +6068,17 @@
     <row r="1" spans="1:7">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="76" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="90" t="s">
+      <c r="E1" s="77"/>
+      <c r="F1" s="76" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="91"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
@@ -5960,94 +6090,94 @@
       <c r="C2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="50" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="74"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="66"/>
+      <c r="B4" s="21" t="s">
         <v>150</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="50" t="s">
+      <c r="E4" s="51"/>
+      <c r="F4" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="74"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="49">
         <v>6</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="51">
         <v>6</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="49">
         <v>7</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="51">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="74"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="66"/>
+      <c r="B6" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="51">
         <v>5</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="51">
         <v>4</v>
       </c>
     </row>
@@ -6067,7 +6197,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6083,45 +6213,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="108" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="109" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>78</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -6144,211 +6274,211 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="29" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="29" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="106"/>
-      <c r="B5" s="112" t="s">
+      <c r="A5" s="92"/>
+      <c r="B5" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="98"/>
+      <c r="D5" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <v>22</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="29">
         <v>22</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <v>22</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>22</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="29">
         <v>13</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="29">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="106"/>
-      <c r="B6" s="102" t="s">
+      <c r="A6" s="92"/>
+      <c r="B6" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="29" t="s">
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="29" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="106"/>
-      <c r="B7" s="93" t="s">
+      <c r="A7" s="92"/>
+      <c r="B7" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="33" t="s">
+      <c r="C7" s="80"/>
+      <c r="D7" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="K7" s="30" t="s">
+      <c r="K7" s="29" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="106"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="34" t="s">
+      <c r="A8" s="92"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="29" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="106"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="33" t="s">
+      <c r="A9" s="92"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>345</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="29">
         <v>567</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="29">
         <v>2100</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>452</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="29">
         <v>643</v>
       </c>
-      <c r="K9" s="30">
+      <c r="K9" s="29">
         <v>783</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="107"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="33" t="s">
+      <c r="A10" s="93"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>0.45</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <v>0.65</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <v>0.67</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="31">
         <v>0.45</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="31">
         <v>0.34</v>
       </c>
     </row>
@@ -6376,7 +6506,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6406,7 +6536,7 @@
       <c r="F1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6429,7 +6559,7 @@
       <c r="F2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>92</v>
       </c>
     </row>
@@ -6452,39 +6582,39 @@
       <c r="F3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="16"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="17"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="17"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="101" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -6494,10 +6624,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="116"/>
+      <c r="A8" s="102"/>
       <c r="B8" s="4" t="s">
         <v>82</v>
       </c>
@@ -6505,41 +6635,41 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="103" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>99</v>
       </c>
       <c r="D9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="27" t="b">
+      <c r="E9" s="26" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="118"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="104"/>
+      <c r="B10" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
@@ -6605,7 +6735,7 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>91</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -6621,7 +6751,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="17"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
@@ -6641,7 +6771,7 @@
       <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>92</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -6659,7 +6789,7 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
@@ -6671,7 +6801,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="17"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
@@ -6681,7 +6811,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -6702,7 +6832,7 @@
         <f>E14</f>
         <v>V2.2</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>93</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -6724,7 +6854,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="17"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
@@ -6738,16 +6868,16 @@
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>99</v>
       </c>
       <c r="E9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="27" t="b">
+      <c r="G9" s="26" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="7">
@@ -6755,7 +6885,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>98</v>
       </c>
     </row>
@@ -6792,27 +6922,28 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -6825,19 +6956,19 @@
       <c r="C2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="150" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6848,7 +6979,7 @@
       <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="106" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -6874,7 +7005,7 @@
       <c r="B4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="121"/>
+      <c r="C4" s="107"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -6898,7 +7029,7 @@
       <c r="B5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="122"/>
+      <c r="C5" s="108"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -6918,13 +7049,13 @@
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>99</v>
       </c>
       <c r="F6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="27" t="b">
+      <c r="G6" s="26" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="7">

</xml_diff>

<commit_message>
test 5 scenario by matcher and unmatcher
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C88E739-0F26-46AC-A9FE-43001BE45FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8939F445-87D7-4B1D-A404-EC18C76B6241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="240">
   <si>
     <t>Role</t>
   </si>
@@ -707,9 +707,6 @@
     <t>Scenario5:Expected</t>
   </si>
   <si>
-    <t>Scenario6:TestResult</t>
-  </si>
-  <si>
     <t>SBT2.1.1</t>
   </si>
   <si>
@@ -765,6 +762,12 @@
   </si>
   <si>
     <t>notexisted</t>
+  </si>
+  <si>
+    <t>Scenario5B:TestResult</t>
+  </si>
+  <si>
+    <t>Scenario5C:TestResult@V0.2</t>
   </si>
 </sst>
 </file>
@@ -2034,7 +2037,7 @@
         <v>217</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2432,13 +2435,13 @@
         <v>17</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -2474,13 +2477,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M12" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30">
@@ -3455,7 +3458,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D4" s="8" t="str">
         <f>C4</f>
@@ -3697,10 +3700,10 @@
         <v>141</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>141</v>
@@ -4426,7 +4429,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4483,19 +4486,19 @@
         <v>218</v>
       </c>
       <c r="L1" s="53" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="M1" s="53" t="s">
         <v>216</v>
       </c>
       <c r="N1" s="53" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="O1" s="55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P1" s="55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1">
@@ -4542,7 +4545,7 @@
         <v>156</v>
       </c>
       <c r="O2" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P2" s="60" t="s">
         <v>156</v>
@@ -4554,7 +4557,7 @@
       </c>
       <c r="B3" s="93"/>
       <c r="C3" s="57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="58" t="s">
         <v>145</v>
@@ -4591,7 +4594,7 @@
       </c>
       <c r="O3" s="61"/>
       <c r="P3" s="61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="31.5">
@@ -4600,7 +4603,7 @@
       </c>
       <c r="B4" s="93"/>
       <c r="C4" s="62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" s="58" t="s">
         <v>145</v>
@@ -4642,7 +4645,7 @@
       </c>
       <c r="B5" s="94"/>
       <c r="C5" s="62" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="58" t="s">
         <v>145</v>
@@ -4654,14 +4657,14 @@
         <v>214</v>
       </c>
       <c r="G5" s="60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H5" s="60"/>
       <c r="I5" s="60"/>
       <c r="J5" s="60"/>
       <c r="K5" s="60"/>
       <c r="L5" s="60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M5" s="60" t="s">
         <v>215</v>
@@ -4759,7 +4762,7 @@
         <v>17</v>
       </c>
       <c r="N7" s="60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O7" s="60" t="s">
         <v>17</v>
@@ -4807,7 +4810,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N8" s="60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O8" s="60">
         <v>4.4000000000000004</v>
@@ -4974,13 +4977,13 @@
       </c>
       <c r="B13" s="84"/>
       <c r="C13" s="64" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F13" s="89" t="s">
         <v>85</v>
@@ -5112,7 +5115,7 @@
       <c r="A19" s="87"/>
       <c r="B19" s="84"/>
       <c r="C19" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="88"/>
       <c r="E19" s="97"/>
@@ -5897,7 +5900,7 @@
       </c>
       <c r="G1" s="109"/>
       <c r="H1" s="108" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I1" s="109"/>
     </row>
@@ -5953,7 +5956,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I3" s="50" t="s">
         <v>206</v>
@@ -5977,13 +5980,13 @@
         <v>204</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" s="48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">

</xml_diff>

<commit_message>
change color in excelbdd excel file
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10C6C64-80C1-4DCC-8785-F42F3212467B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795667B4-174D-4F52-B00B-7332C2BD4E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" firstSheet="1" activeTab="10" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="243">
   <si>
     <t>Role</t>
   </si>
@@ -707,9 +707,6 @@
     <t>Scenario5:Expected</t>
   </si>
   <si>
-    <t>Scenario6:TestResult</t>
-  </si>
-  <si>
     <t>SBT2.1.1</t>
   </si>
   <si>
@@ -762,6 +759,24 @@
   </si>
   <si>
     <t>unlimited count of blank parameters</t>
+  </si>
+  <si>
+    <t>notexisted</t>
+  </si>
+  <si>
+    <t>Scenario5B:TestResult</t>
+  </si>
+  <si>
+    <t>Scenario5C:TestResult@V0.2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -849,7 +864,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -924,6 +939,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1102,7 +1123,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1502,6 +1523,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1966,10 +1993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2031,7 +2059,7 @@
         <v>217</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2429,13 +2457,13 @@
         <v>17</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -2471,13 +2499,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M12" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30">
@@ -2818,6 +2846,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9F3738-1988-486F-BE99-D486460FE985}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3017,10 +3046,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3126,50 +3156,50 @@
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="8" t="str">
+      <c r="D3" s="150" t="str">
         <f>C3</f>
         <v>V1.1</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8" t="str">
+      <c r="G3" s="150" t="str">
         <f>F3</f>
         <v>V1.2</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="8" t="str">
+      <c r="J3" s="150" t="str">
         <f>I3</f>
         <v>V1.3</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="8" t="str">
+      <c r="M3" s="150" t="str">
         <f>L3</f>
         <v>V1.4</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="8" t="str">
+      <c r="P3" s="150" t="str">
         <f>O3</f>
         <v>V1.5</v>
       </c>
@@ -3184,50 +3214,50 @@
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="8" t="str">
+      <c r="D4" s="150" t="str">
         <f t="shared" ref="D4:D6" si="0">C4</f>
         <v>V2.1</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8" t="str">
+      <c r="G4" s="150" t="str">
         <f t="shared" ref="G4:G6" si="1">F4</f>
         <v>V2.2</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="8" t="str">
+      <c r="J4" s="150" t="str">
         <f t="shared" ref="J4:J6" si="2">I4</f>
         <v>V2.3</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="150" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="8" t="str">
+      <c r="M4" s="150" t="str">
         <f t="shared" ref="M4:M6" si="3">L4</f>
         <v>V2.4</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="8" t="str">
+      <c r="P4" s="150" t="str">
         <f t="shared" ref="P4" si="4">O4</f>
         <v>V2.5</v>
       </c>
@@ -3242,28 +3272,28 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="150"/>
       <c r="E5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="150"/>
+      <c r="G5" s="150"/>
       <c r="H5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="150"/>
+      <c r="J5" s="150"/>
       <c r="K5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
       <c r="N5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="O5" s="150"/>
+      <c r="P5" s="150"/>
       <c r="Q5" s="8" t="s">
         <v>141</v>
       </c>
@@ -3275,50 +3305,50 @@
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="151" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="8" t="str">
+      <c r="D6" s="150" t="str">
         <f t="shared" si="0"/>
         <v>2021/4/30</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="8" t="b">
+      <c r="F6" s="150" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="8" t="b">
+      <c r="G6" s="150" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I6" s="25" t="b">
+      <c r="I6" s="152" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="8" t="b">
+      <c r="J6" s="150" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="153">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="150">
         <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="153">
         <v>5.4</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="150">
         <f t="shared" ref="P6" si="5">O6</f>
         <v>5.4</v>
       </c>
@@ -3341,6 +3371,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD4D131-69ED-4813-926B-7E95E2B369DB}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3452,7 +3483,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D4" s="8" t="str">
         <f>C4</f>
@@ -3694,10 +3725,10 @@
         <v>141</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>141</v>
@@ -3717,10 +3748,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27202F44-224C-40C0-ACC3-02135A9560D7}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3738,6 +3770,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
       <c r="D1" s="34" t="s">
         <v>142</v>
       </c>
@@ -3851,60 +3892,60 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="8" t="str">
+      <c r="F3" s="150" t="str">
         <f>E3</f>
         <v>V1.1</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="8" t="str">
+      <c r="I3" s="150" t="str">
         <f>H3</f>
         <v>V1.2</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="8" t="str">
+      <c r="L3" s="150" t="str">
         <f>K3</f>
         <v>V1.3</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="8" t="str">
+      <c r="O3" s="150" t="str">
         <f>N3</f>
         <v>V1.4</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="R3" s="8" t="str">
+      <c r="R3" s="150" t="str">
         <f>Q3</f>
         <v>V1.5</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="8" t="str">
+      <c r="U3" s="150" t="str">
         <f>T3</f>
         <v>V1.1</v>
       </c>
@@ -3923,60 +3964,60 @@
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="8" t="str">
+      <c r="F4" s="150" t="str">
         <f t="shared" ref="F4:F6" si="0">E4</f>
         <v>V2.1</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="8" t="str">
+      <c r="I4" s="150" t="str">
         <f t="shared" ref="I4:I6" si="1">H4</f>
         <v>V2.2</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="8" t="str">
+      <c r="L4" s="150" t="str">
         <f t="shared" ref="L4:L6" si="2">K4</f>
         <v>V2.3</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="150" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="8" t="str">
+      <c r="O4" s="150" t="str">
         <f t="shared" ref="O4:O6" si="3">N4</f>
         <v>V2.4</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="R4" s="8" t="str">
+      <c r="R4" s="150" t="str">
         <f t="shared" ref="R4" si="4">Q4</f>
         <v>V2.5</v>
       </c>
       <c r="S4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="T4" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="8" t="str">
+      <c r="U4" s="150" t="str">
         <f t="shared" ref="U4" si="5">T4</f>
         <v>V2.1</v>
       </c>
@@ -3995,33 +4036,33 @@
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="150"/>
+      <c r="F5" s="150"/>
       <c r="G5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="H5" s="150"/>
+      <c r="I5" s="150"/>
       <c r="J5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150"/>
       <c r="M5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="N5" s="150"/>
+      <c r="O5" s="150"/>
       <c r="P5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="Q5" s="150"/>
+      <c r="R5" s="150"/>
       <c r="S5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="T5" s="150"/>
+      <c r="U5" s="150"/>
       <c r="V5" s="8" t="s">
         <v>141</v>
       </c>
@@ -4037,60 +4078,60 @@
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="151" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="8" t="str">
+      <c r="F6" s="150" t="str">
         <f t="shared" si="0"/>
         <v>2021/4/30</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="8" t="b">
+      <c r="H6" s="150" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="8" t="b">
+      <c r="I6" s="150" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K6" s="25" t="b">
+      <c r="K6" s="152" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="8" t="b">
+      <c r="L6" s="150" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="153">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="150">
         <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="153">
         <v>4.5</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="150">
         <f t="shared" ref="R6" si="6">Q6</f>
         <v>4.5</v>
       </c>
       <c r="S6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T6" s="26" t="s">
+      <c r="T6" s="151" t="s">
         <v>96</v>
       </c>
-      <c r="U6" s="8" t="str">
+      <c r="U6" s="150" t="str">
         <f t="shared" ref="U6" si="7">T6</f>
         <v>2021/4/30</v>
       </c>
@@ -4115,6 +4156,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFF208A-E752-404F-A219-18F91B0322F1}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4333,6 +4375,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ACBBF6-9F77-42E6-ADBF-E42E08CDCCFD}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4420,10 +4463,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93BB7E4-E9BF-490F-8356-65B5D0024489}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4480,19 +4524,19 @@
         <v>218</v>
       </c>
       <c r="L1" s="53" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="M1" s="53" t="s">
         <v>216</v>
       </c>
       <c r="N1" s="53" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="O1" s="55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P1" s="55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1">
@@ -4539,7 +4583,7 @@
         <v>156</v>
       </c>
       <c r="O2" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P2" s="60" t="s">
         <v>156</v>
@@ -4551,7 +4595,7 @@
       </c>
       <c r="B3" s="93"/>
       <c r="C3" s="57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="58" t="s">
         <v>145</v>
@@ -4588,7 +4632,7 @@
       </c>
       <c r="O3" s="61"/>
       <c r="P3" s="61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="31.5">
@@ -4597,7 +4641,7 @@
       </c>
       <c r="B4" s="93"/>
       <c r="C4" s="62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" s="58" t="s">
         <v>145</v>
@@ -4639,7 +4683,7 @@
       </c>
       <c r="B5" s="94"/>
       <c r="C5" s="62" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="58" t="s">
         <v>145</v>
@@ -4650,13 +4694,15 @@
       <c r="F5" s="63" t="s">
         <v>214</v>
       </c>
-      <c r="G5" s="60"/>
+      <c r="G5" s="60" t="s">
+        <v>237</v>
+      </c>
       <c r="H5" s="60"/>
       <c r="I5" s="60"/>
       <c r="J5" s="60"/>
       <c r="K5" s="60"/>
       <c r="L5" s="60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M5" s="60" t="s">
         <v>215</v>
@@ -4754,7 +4800,7 @@
         <v>17</v>
       </c>
       <c r="N7" s="60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O7" s="60" t="s">
         <v>17</v>
@@ -4802,7 +4848,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N8" s="60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O8" s="60">
         <v>4.4000000000000004</v>
@@ -4969,13 +5015,13 @@
       </c>
       <c r="B13" s="84"/>
       <c r="C13" s="64" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F13" s="89" t="s">
         <v>85</v>
@@ -5107,7 +5153,7 @@
       <c r="A19" s="87"/>
       <c r="B19" s="84"/>
       <c r="C19" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="88"/>
       <c r="E19" s="97"/>
@@ -5235,6 +5281,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A3:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5858,6 +5905,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE4E5E2-8FAC-4516-9FEA-053724A7E1DD}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5892,7 +5940,7 @@
       </c>
       <c r="G1" s="109"/>
       <c r="H1" s="108" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I1" s="109"/>
     </row>
@@ -5948,7 +5996,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I3" s="50" t="s">
         <v>206</v>
@@ -5972,13 +6020,13 @@
         <v>204</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" s="48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
@@ -6041,6 +6089,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DB7B63-E032-433E-B0E0-E6E5C56D92F2}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6187,6 +6236,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -6496,10 +6546,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5657C2-106C-47C7-BF16-329C2F267F09}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6677,6 +6728,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A494DA1E-3A4D-414E-886D-A717DFF21DE7}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6864,6 +6916,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3FD2D2-D808-401C-A638-EED224C6394A}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
deal with default sheet
</commit_message>
<xml_diff>
--- a/BDDExcel/ExcelBDD.xlsx
+++ b/BDDExcel/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ExcelBDD\BDDExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795667B4-174D-4F52-B00B-7332C2BD4E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E58323-9B52-4DC0-B369-F6692EF31959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" firstSheet="1" activeTab="10" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" firstSheet="2" activeTab="11" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecificationByExample" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="244">
   <si>
     <t>Role</t>
   </si>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>ScenarioTable</t>
   </si>
 </sst>
 </file>
@@ -1287,248 +1290,248 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2066,7 +2069,7 @@
       <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="82" t="s">
         <v>207</v>
       </c>
       <c r="C2" s="21" t="s">
@@ -2110,7 +2113,7 @@
       <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
+      <c r="B3" s="83"/>
       <c r="C3" s="21" t="s">
         <v>147</v>
       </c>
@@ -2152,7 +2155,7 @@
       <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
@@ -2194,7 +2197,7 @@
       <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="79"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="21" t="s">
         <v>27</v>
       </c>
@@ -2234,7 +2237,7 @@
     </row>
     <row r="6" spans="1:14" ht="30">
       <c r="A6" s="20"/>
-      <c r="B6" s="79"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="24" t="s">
         <v>87</v>
       </c>
@@ -2272,7 +2275,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="20"/>
-      <c r="B7" s="79"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="24" t="s">
         <v>212</v>
       </c>
@@ -2300,7 +2303,7 @@
       <c r="A8" s="20">
         <v>5</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="43" t="s">
         <v>175</v>
       </c>
@@ -2342,7 +2345,7 @@
       <c r="A9" s="20">
         <v>6</v>
       </c>
-      <c r="B9" s="80"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="45" t="s">
         <v>176</v>
       </c>
@@ -2384,7 +2387,7 @@
       <c r="A10" s="20">
         <v>7</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="85" t="s">
         <v>168</v>
       </c>
       <c r="C10" s="21" t="s">
@@ -2428,7 +2431,7 @@
       <c r="A11" s="20">
         <v>8</v>
       </c>
-      <c r="B11" s="82"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="21" t="s">
         <v>31</v>
       </c>
@@ -2470,7 +2473,7 @@
       <c r="A12" s="20">
         <v>9</v>
       </c>
-      <c r="B12" s="82"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="21" t="s">
         <v>34</v>
       </c>
@@ -2512,7 +2515,7 @@
       <c r="A13" s="20">
         <v>10</v>
       </c>
-      <c r="B13" s="82"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="22" t="s">
         <v>68</v>
       </c>
@@ -2554,7 +2557,7 @@
       <c r="A14" s="20">
         <v>11</v>
       </c>
-      <c r="B14" s="82"/>
+      <c r="B14" s="86"/>
       <c r="C14" s="22" t="s">
         <v>69</v>
       </c>
@@ -2596,7 +2599,7 @@
       <c r="A15" s="20">
         <v>12</v>
       </c>
-      <c r="B15" s="82"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="22" t="s">
         <v>66</v>
       </c>
@@ -2622,7 +2625,7 @@
       <c r="A16" s="20">
         <v>13</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="21" t="s">
         <v>81</v>
       </c>
@@ -2645,20 +2648,20 @@
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" ht="45">
-      <c r="A17" s="71">
+      <c r="A17" s="75">
         <v>14</v>
       </c>
-      <c r="B17" s="82"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="74" t="s">
+      <c r="D17" s="78" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="F17" s="75" t="s">
+      <c r="F17" s="79" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="7">
@@ -2687,16 +2690,16 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="72"/>
-      <c r="B18" s="82"/>
+      <c r="A18" s="76"/>
+      <c r="B18" s="86"/>
       <c r="C18" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="74"/>
+      <c r="D18" s="78"/>
       <c r="E18" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="76"/>
+      <c r="F18" s="80"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -2707,16 +2710,16 @@
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="72"/>
-      <c r="B19" s="82"/>
+      <c r="A19" s="76"/>
+      <c r="B19" s="86"/>
       <c r="C19" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="74"/>
+      <c r="D19" s="78"/>
       <c r="E19" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="F19" s="76"/>
+      <c r="F19" s="80"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2727,16 +2730,16 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="73"/>
-      <c r="B20" s="82"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="74"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="F20" s="77"/>
+      <c r="F20" s="81"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2750,7 +2753,7 @@
       <c r="A21" s="23">
         <v>16</v>
       </c>
-      <c r="B21" s="82"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="24" t="s">
         <v>36</v>
       </c>
@@ -2792,7 +2795,7 @@
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="B22" s="83"/>
+      <c r="B22" s="87"/>
       <c r="C22" s="39" t="s">
         <v>160</v>
       </c>
@@ -2863,42 +2866,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="137" t="s">
+      <c r="B1" s="147"/>
+      <c r="C1" s="141" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="137"/>
+      <c r="D1" s="141"/>
       <c r="E1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="141" t="s">
+      <c r="F1" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="146" t="s">
+      <c r="B2" s="147"/>
+      <c r="C2" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="146"/>
+      <c r="D2" s="150"/>
       <c r="E2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="144" t="s">
+      <c r="F2" s="148" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="145"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="149"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="12" t="s">
@@ -2930,16 +2933,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="127" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="123" t="s">
+      <c r="C4" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="138" t="s">
+      <c r="D4" s="142" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2959,12 +2962,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="124"/>
+      <c r="A5" s="128"/>
       <c r="B5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="139"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="143"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2982,12 +2985,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="124"/>
+      <c r="A6" s="128"/>
       <c r="B6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="140"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="144"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2997,7 +3000,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="125"/>
+      <c r="A7" s="129"/>
       <c r="B7" s="9" t="s">
         <v>60</v>
       </c>
@@ -3049,9 +3052,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:P6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3067,34 +3068,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
+      <c r="A1">
+        <v>1</v>
+      </c>
       <c r="B1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="109"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="108" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="109"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="108" t="s">
+      <c r="G1" s="113"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="109"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="148" t="s">
+      <c r="J1" s="113"/>
+      <c r="K1" s="151"/>
+      <c r="L1" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
-      <c r="O1" s="108" t="s">
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="112" t="s">
         <v>127</v>
       </c>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="147"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="151"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -3156,50 +3160,50 @@
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="150" t="s">
+      <c r="C3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="150" t="str">
+      <c r="D3" s="71" t="str">
         <f>C3</f>
         <v>V1.1</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="150" t="s">
+      <c r="F3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="150" t="str">
+      <c r="G3" s="71" t="str">
         <f>F3</f>
         <v>V1.2</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="150" t="s">
+      <c r="I3" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="150" t="str">
+      <c r="J3" s="71" t="str">
         <f>I3</f>
         <v>V1.3</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L3" s="150" t="s">
+      <c r="L3" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="150" t="str">
+      <c r="M3" s="71" t="str">
         <f>L3</f>
         <v>V1.4</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O3" s="150" t="s">
+      <c r="O3" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="150" t="str">
+      <c r="P3" s="71" t="str">
         <f>O3</f>
         <v>V1.5</v>
       </c>
@@ -3214,50 +3218,50 @@
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="150" t="str">
+      <c r="D4" s="71" t="str">
         <f t="shared" ref="D4:D6" si="0">C4</f>
         <v>V2.1</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="150" t="s">
+      <c r="F4" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="150" t="str">
+      <c r="G4" s="71" t="str">
         <f t="shared" ref="G4:G6" si="1">F4</f>
         <v>V2.2</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="150" t="s">
+      <c r="I4" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="150" t="str">
+      <c r="J4" s="71" t="str">
         <f t="shared" ref="J4:J6" si="2">I4</f>
         <v>V2.3</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L4" s="150" t="s">
+      <c r="L4" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="150" t="str">
+      <c r="M4" s="71" t="str">
         <f t="shared" ref="M4:M6" si="3">L4</f>
         <v>V2.4</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O4" s="150" t="s">
+      <c r="O4" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="150" t="str">
+      <c r="P4" s="71" t="str">
         <f t="shared" ref="P4" si="4">O4</f>
         <v>V2.5</v>
       </c>
@@ -3272,28 +3276,28 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="150"/>
-      <c r="D5" s="150"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="150"/>
-      <c r="G5" s="150"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I5" s="150"/>
-      <c r="J5" s="150"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
       <c r="K5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L5" s="150"/>
-      <c r="M5" s="150"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
       <c r="N5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="150"/>
-      <c r="P5" s="150"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="71"/>
       <c r="Q5" s="8" t="s">
         <v>141</v>
       </c>
@@ -3305,50 +3309,50 @@
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="150" t="str">
+      <c r="D6" s="71" t="str">
         <f t="shared" si="0"/>
         <v>2021/4/30</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="150" t="b">
+      <c r="F6" s="71" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="150" t="b">
+      <c r="G6" s="71" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I6" s="152" t="b">
+      <c r="I6" s="73" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="150" t="b">
+      <c r="J6" s="71" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L6" s="153">
+      <c r="L6" s="74">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M6" s="150">
+      <c r="M6" s="71">
         <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O6" s="153">
+      <c r="O6" s="74">
         <v>5.4</v>
       </c>
-      <c r="P6" s="150">
+      <c r="P6" s="71">
         <f t="shared" ref="P6" si="5">O6</f>
         <v>5.4</v>
       </c>
@@ -3374,8 +3378,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3391,29 +3395,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>243</v>
+      </c>
       <c r="B1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="109"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="108" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="109"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="108" t="s">
+      <c r="G1" s="113"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="109"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="148" t="s">
+      <c r="J1" s="113"/>
+      <c r="K1" s="151"/>
+      <c r="L1" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3752,7 +3759,7 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3782,36 +3789,36 @@
       <c r="D1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="109"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="108" t="s">
+      <c r="F1" s="113"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="109"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="108" t="s">
+      <c r="I1" s="113"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="110" t="s">
+      <c r="L1" s="113"/>
+      <c r="M1" s="151"/>
+      <c r="N1" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="108" t="s">
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="112" t="s">
         <v>127</v>
       </c>
-      <c r="R1" s="109"/>
-      <c r="S1" s="147"/>
-      <c r="T1" s="108" t="s">
+      <c r="R1" s="113"/>
+      <c r="S1" s="151"/>
+      <c r="T1" s="112" t="s">
         <v>159</v>
       </c>
-      <c r="U1" s="109"/>
-      <c r="V1" s="147"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="151"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -3892,60 +3899,60 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="150" t="s">
+      <c r="E3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="150" t="str">
+      <c r="F3" s="71" t="str">
         <f>E3</f>
         <v>V1.1</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="150" t="s">
+      <c r="H3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="150" t="str">
+      <c r="I3" s="71" t="str">
         <f>H3</f>
         <v>V1.2</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K3" s="150" t="s">
+      <c r="K3" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="150" t="str">
+      <c r="L3" s="71" t="str">
         <f>K3</f>
         <v>V1.3</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="150" t="s">
+      <c r="N3" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="150" t="str">
+      <c r="O3" s="71" t="str">
         <f>N3</f>
         <v>V1.4</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q3" s="150" t="s">
+      <c r="Q3" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="R3" s="150" t="str">
+      <c r="R3" s="71" t="str">
         <f>Q3</f>
         <v>V1.5</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T3" s="150" t="s">
+      <c r="T3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="150" t="str">
+      <c r="U3" s="71" t="str">
         <f>T3</f>
         <v>V1.1</v>
       </c>
@@ -3964,60 +3971,60 @@
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="150" t="s">
+      <c r="E4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="150" t="str">
+      <c r="F4" s="71" t="str">
         <f t="shared" ref="F4:F6" si="0">E4</f>
         <v>V2.1</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="150" t="s">
+      <c r="H4" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="150" t="str">
+      <c r="I4" s="71" t="str">
         <f t="shared" ref="I4:I6" si="1">H4</f>
         <v>V2.2</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K4" s="150" t="s">
+      <c r="K4" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="150" t="str">
+      <c r="L4" s="71" t="str">
         <f t="shared" ref="L4:L6" si="2">K4</f>
         <v>V2.3</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="150" t="str">
+      <c r="O4" s="71" t="str">
         <f t="shared" ref="O4:O6" si="3">N4</f>
         <v>V2.4</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q4" s="150" t="s">
+      <c r="Q4" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="R4" s="150" t="str">
+      <c r="R4" s="71" t="str">
         <f t="shared" ref="R4" si="4">Q4</f>
         <v>V2.5</v>
       </c>
       <c r="S4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T4" s="150" t="s">
+      <c r="T4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="150" t="str">
+      <c r="U4" s="71" t="str">
         <f t="shared" ref="U4" si="5">T4</f>
         <v>V2.1</v>
       </c>
@@ -4036,33 +4043,33 @@
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="150"/>
-      <c r="F5" s="150"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="150"/>
-      <c r="I5" s="150"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
       <c r="J5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K5" s="150"/>
-      <c r="L5" s="150"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
       <c r="M5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N5" s="150"/>
-      <c r="O5" s="150"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="71"/>
       <c r="P5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q5" s="150"/>
-      <c r="R5" s="150"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
       <c r="S5" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T5" s="150"/>
-      <c r="U5" s="150"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="71"/>
       <c r="V5" s="8" t="s">
         <v>141</v>
       </c>
@@ -4078,60 +4085,60 @@
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="151" t="s">
+      <c r="E6" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="150" t="str">
+      <c r="F6" s="71" t="str">
         <f t="shared" si="0"/>
         <v>2021/4/30</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="150" t="b">
+      <c r="H6" s="71" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="150" t="b">
+      <c r="I6" s="71" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K6" s="152" t="b">
+      <c r="K6" s="73" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="150" t="b">
+      <c r="L6" s="71" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N6" s="153">
+      <c r="N6" s="74">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O6" s="150">
+      <c r="O6" s="71">
         <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q6" s="153">
+      <c r="Q6" s="74">
         <v>4.5</v>
       </c>
-      <c r="R6" s="150">
+      <c r="R6" s="71">
         <f t="shared" ref="R6" si="6">Q6</f>
         <v>4.5</v>
       </c>
       <c r="S6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="T6" s="151" t="s">
+      <c r="T6" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="U6" s="150" t="str">
+      <c r="U6" s="71" t="str">
         <f t="shared" ref="U6" si="7">T6</f>
         <v>2021/4/30</v>
       </c>
@@ -4160,7 +4167,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD13"/>
+      <selection activeCell="C3" sqref="C3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4175,24 +4182,24 @@
       <c r="B1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="109"/>
-      <c r="E1" s="108" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="109"/>
-      <c r="G1" s="108" t="s">
+      <c r="F1" s="113"/>
+      <c r="G1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="109"/>
-      <c r="I1" s="148" t="s">
+      <c r="H1" s="113"/>
+      <c r="I1" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="149"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="109"/>
+      <c r="J1" s="153"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
@@ -4466,8 +4473,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4543,7 +4550,7 @@
       <c r="A2" s="56">
         <v>1</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="96" t="s">
         <v>207</v>
       </c>
       <c r="C2" s="57" t="s">
@@ -4593,7 +4600,7 @@
       <c r="A3" s="56">
         <v>2</v>
       </c>
-      <c r="B3" s="93"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="57" t="s">
         <v>229</v>
       </c>
@@ -4639,7 +4646,7 @@
       <c r="A4" s="56">
         <v>3</v>
       </c>
-      <c r="B4" s="93"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="62" t="s">
         <v>230</v>
       </c>
@@ -4681,7 +4688,7 @@
       <c r="A5" s="56">
         <v>4</v>
       </c>
-      <c r="B5" s="94"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="62" t="s">
         <v>231</v>
       </c>
@@ -4715,7 +4722,7 @@
       <c r="A6" s="56">
         <v>5</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="88" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="64" t="s">
@@ -4765,7 +4772,7 @@
       <c r="A7" s="56">
         <v>6</v>
       </c>
-      <c r="B7" s="84"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="64" t="s">
         <v>31</v>
       </c>
@@ -4813,7 +4820,7 @@
       <c r="A8" s="56">
         <v>7</v>
       </c>
-      <c r="B8" s="84"/>
+      <c r="B8" s="88"/>
       <c r="C8" s="64" t="s">
         <v>34</v>
       </c>
@@ -4861,7 +4868,7 @@
       <c r="A9" s="56">
         <v>8</v>
       </c>
-      <c r="B9" s="84"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="64" t="s">
         <v>68</v>
       </c>
@@ -4909,7 +4916,7 @@
       <c r="A10" s="56">
         <v>9</v>
       </c>
-      <c r="B10" s="84"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="64" t="s">
         <v>69</v>
       </c>
@@ -4957,7 +4964,7 @@
       <c r="A11" s="56">
         <v>10</v>
       </c>
-      <c r="B11" s="84"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="64" t="s">
         <v>66</v>
       </c>
@@ -4985,7 +4992,7 @@
       <c r="A12" s="56">
         <v>11</v>
       </c>
-      <c r="B12" s="84"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="64" t="s">
         <v>81</v>
       </c>
@@ -5010,20 +5017,20 @@
       <c r="P12" s="60"/>
     </row>
     <row r="13" spans="1:16" ht="47.25">
-      <c r="A13" s="85">
+      <c r="A13" s="89">
         <v>12</v>
       </c>
-      <c r="B13" s="84"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="64" t="s">
         <v>235</v>
       </c>
-      <c r="D13" s="88" t="s">
+      <c r="D13" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="95" t="s">
+      <c r="E13" s="99" t="s">
         <v>234</v>
       </c>
-      <c r="F13" s="89" t="s">
+      <c r="F13" s="93" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="60">
@@ -5058,14 +5065,14 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="31.5">
-      <c r="A14" s="86"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="90"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="94"/>
       <c r="G14" s="60"/>
       <c r="H14" s="60"/>
       <c r="I14" s="60"/>
@@ -5078,12 +5085,12 @@
       <c r="P14" s="60"/>
     </row>
     <row r="15" spans="1:16" ht="15.75">
-      <c r="A15" s="86"/>
-      <c r="B15" s="84"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="64"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="90"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="60"/>
       <c r="H15" s="60"/>
       <c r="I15" s="60"/>
@@ -5096,14 +5103,14 @@
       <c r="P15" s="60"/>
     </row>
     <row r="16" spans="1:16" ht="15.75">
-      <c r="A16" s="86"/>
-      <c r="B16" s="84"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="88"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="90"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="94"/>
       <c r="G16" s="60"/>
       <c r="H16" s="60"/>
       <c r="I16" s="60"/>
@@ -5116,11 +5123,11 @@
       <c r="P16" s="60"/>
     </row>
     <row r="17" spans="1:16" ht="15.75">
-      <c r="A17" s="86"/>
-      <c r="B17" s="84"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="90"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="88"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="94"/>
       <c r="G17" s="60"/>
       <c r="H17" s="60"/>
       <c r="I17" s="60"/>
@@ -5133,11 +5140,11 @@
       <c r="P17" s="60"/>
     </row>
     <row r="18" spans="1:16" ht="15.75">
-      <c r="A18" s="86"/>
-      <c r="B18" s="84"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="90"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="88"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="94"/>
       <c r="G18" s="60"/>
       <c r="H18" s="60"/>
       <c r="I18" s="60"/>
@@ -5150,14 +5157,14 @@
       <c r="P18" s="60"/>
     </row>
     <row r="19" spans="1:16" ht="15.75">
-      <c r="A19" s="87"/>
-      <c r="B19" s="84"/>
+      <c r="A19" s="91"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="D19" s="88"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="91"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="95"/>
       <c r="G19" s="60"/>
       <c r="H19" s="60"/>
       <c r="I19" s="60"/>
@@ -5173,7 +5180,7 @@
       <c r="A20" s="58">
         <v>13</v>
       </c>
-      <c r="B20" s="84"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="67" t="s">
         <v>36</v>
       </c>
@@ -5221,7 +5228,7 @@
       <c r="A21" s="68">
         <v>14</v>
       </c>
-      <c r="B21" s="84"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="69" t="s">
         <v>160</v>
       </c>
@@ -5305,41 +5312,41 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="109" t="s">
         <v>155</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G3" s="98" t="s">
+      <c r="G3" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="98" t="s">
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="104"/>
-      <c r="B4" s="104"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
+      <c r="A4" s="108"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
       <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
@@ -5363,7 +5370,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="104" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -5401,7 +5408,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100"/>
+      <c r="A6" s="104"/>
       <c r="B6" s="21" t="s">
         <v>147</v>
       </c>
@@ -5437,7 +5444,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="100"/>
+      <c r="A7" s="104"/>
       <c r="B7" s="21" t="s">
         <v>25</v>
       </c>
@@ -5473,7 +5480,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="100"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="21" t="s">
         <v>27</v>
       </c>
@@ -5509,7 +5516,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="100"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="21" t="s">
         <v>175</v>
       </c>
@@ -5545,7 +5552,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="100"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="40" t="s">
         <v>176</v>
       </c>
@@ -5581,7 +5588,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="106" t="s">
         <v>168</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -5613,7 +5620,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="102"/>
+      <c r="A12" s="106"/>
       <c r="B12" s="21" t="s">
         <v>148</v>
       </c>
@@ -5649,7 +5656,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="102"/>
+      <c r="A13" s="106"/>
       <c r="B13" s="21" t="s">
         <v>149</v>
       </c>
@@ -5681,7 +5688,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="102"/>
+      <c r="A14" s="106"/>
       <c r="B14" s="21" t="s">
         <v>150</v>
       </c>
@@ -5713,7 +5720,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="102"/>
+      <c r="A15" s="106"/>
       <c r="B15" s="22" t="s">
         <v>151</v>
       </c>
@@ -5749,8 +5756,8 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="102"/>
-      <c r="B16" s="101" t="s">
+      <c r="A16" s="106"/>
+      <c r="B16" s="105" t="s">
         <v>172</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -5787,8 +5794,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="102"/>
-      <c r="B17" s="101"/>
+      <c r="A17" s="106"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="23" t="s">
         <v>5</v>
       </c>
@@ -5823,8 +5830,8 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="102"/>
-      <c r="B18" s="101"/>
+      <c r="A18" s="106"/>
+      <c r="B18" s="105"/>
       <c r="C18" s="23" t="s">
         <v>5</v>
       </c>
@@ -5849,8 +5856,8 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="102"/>
-      <c r="B19" s="101"/>
+      <c r="A19" s="106"/>
+      <c r="B19" s="105"/>
       <c r="C19" s="23" t="s">
         <v>5</v>
       </c>
@@ -5931,18 +5938,18 @@
       <c r="C1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="110" t="s">
+      <c r="D1" s="114" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="110"/>
-      <c r="F1" s="108" t="s">
+      <c r="E1" s="114"/>
+      <c r="F1" s="112" t="s">
         <v>200</v>
       </c>
-      <c r="G1" s="109"/>
-      <c r="H1" s="108" t="s">
+      <c r="G1" s="113"/>
+      <c r="H1" s="112" t="s">
         <v>227</v>
       </c>
-      <c r="I1" s="109"/>
+      <c r="I1" s="113"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
@@ -5974,7 +5981,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="111" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -6003,7 +6010,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="107"/>
+      <c r="A4" s="111"/>
       <c r="B4" s="21" t="s">
         <v>147</v>
       </c>
@@ -6030,7 +6037,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="107"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
@@ -6053,7 +6060,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="107"/>
+      <c r="A6" s="111"/>
       <c r="B6" s="21" t="s">
         <v>27</v>
       </c>
@@ -6113,14 +6120,14 @@
       <c r="C1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="112" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="108" t="s">
+      <c r="E1" s="113"/>
+      <c r="F1" s="112" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="109"/>
+      <c r="G1" s="113"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
@@ -6146,7 +6153,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="111" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -6165,7 +6172,7 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="107"/>
+      <c r="A4" s="111"/>
       <c r="B4" s="21" t="s">
         <v>147</v>
       </c>
@@ -6182,7 +6189,7 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="107"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
@@ -6203,7 +6210,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="107"/>
+      <c r="A6" s="111"/>
       <c r="B6" s="21" t="s">
         <v>27</v>
       </c>
@@ -6256,41 +6263,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="126" t="s">
+      <c r="B1" s="135"/>
+      <c r="C1" s="130" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="127" t="s">
+      <c r="B2" s="136"/>
+      <c r="C2" s="131" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="129"/>
+      <c r="C3" s="133"/>
       <c r="D3" s="12" t="s">
         <v>107</v>
       </c>
@@ -6317,14 +6324,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="119"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="123"/>
       <c r="E4" s="27" t="s">
         <v>99</v>
       </c>
@@ -6348,11 +6355,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="124"/>
-      <c r="B5" s="130" t="s">
+      <c r="A5" s="128"/>
+      <c r="B5" s="134" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="130"/>
+      <c r="C5" s="134"/>
       <c r="D5" s="31" t="s">
         <v>109</v>
       </c>
@@ -6379,12 +6386,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="124"/>
-      <c r="B6" s="120" t="s">
+      <c r="A6" s="128"/>
+      <c r="B6" s="124" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="121"/>
-      <c r="D6" s="122"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="126"/>
       <c r="E6" s="27" t="s">
         <v>105</v>
       </c>
@@ -6408,11 +6415,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="124"/>
-      <c r="B7" s="111" t="s">
+      <c r="A7" s="128"/>
+      <c r="B7" s="115" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="112"/>
+      <c r="C7" s="116"/>
       <c r="D7" s="31" t="s">
         <v>110</v>
       </c>
@@ -6439,9 +6446,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="124"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="114"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="32" t="s">
         <v>116</v>
       </c>
@@ -6468,9 +6475,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="124"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="128"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="31" t="s">
         <v>117</v>
       </c>
@@ -6497,9 +6504,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="125"/>
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
+      <c r="A10" s="129"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="120"/>
       <c r="D10" s="31" t="s">
         <v>118</v>
       </c>
@@ -6658,7 +6665,7 @@
       <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="137" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -6671,7 +6678,7 @@
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="134"/>
+      <c r="A8" s="138"/>
       <c r="B8" s="4" t="s">
         <v>82</v>
       </c>
@@ -6682,7 +6689,7 @@
       <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="135" t="s">
+      <c r="A9" s="139" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -6705,7 +6712,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="136"/>
+      <c r="A10" s="140"/>
       <c r="B10" s="14" t="s">
         <v>82</v>
       </c>
@@ -6933,15 +6940,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -6977,7 +6984,7 @@
       <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="142" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -7003,7 +7010,7 @@
       <c r="B4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="143"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -7027,7 +7034,7 @@
       <c r="B5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="140"/>
+      <c r="C5" s="144"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>